<commit_message>
Ajuste de template de metas para comportar mais metas especificas
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/TEMPLATE_METAS.xlsx
+++ b/src/main/resources/templates/TEMPLATE_METAS.xlsx
@@ -16,7 +16,7 @@
     <sheet name="ESCALONAMENTO" sheetId="6" state="hidden" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'FOLHA METAS'!$A$1:$M$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'FOLHA METAS'!$A$1:$M$46</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -98,6 +98,9 @@
     <t xml:space="preserve">PERFORMANCE DO AVALIADO</t>
   </si>
   <si>
+    <t xml:space="preserve">META EXTRA</t>
+  </si>
+  <si>
     <t xml:space="preserve">METAS QUANTITATIVAS</t>
   </si>
   <si>
@@ -138,9 +141,6 @@
   </si>
   <si>
     <t xml:space="preserve">SUPERIOR IMEDIATO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Após as assinaturas, enviar ORIGINAL e arquivo eletrônico para o Bosi &lt;marcosbosi@cblalimentos.com.br&gt;.</t>
   </si>
   <si>
     <t xml:space="preserve">JAN</t>
@@ -239,7 +239,7 @@
     <numFmt numFmtId="171" formatCode="#,##0"/>
     <numFmt numFmtId="172" formatCode="0.000"/>
   </numFmts>
-  <fonts count="43">
+  <fonts count="40">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -370,6 +370,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="13"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -400,39 +408,7 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="13.5"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="8"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="18"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="13"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -449,6 +425,14 @@
     <font>
       <b val="true"/>
       <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -482,14 +466,6 @@
       <b val="true"/>
       <sz val="8"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -651,7 +627,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="32">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -788,17 +764,6 @@
       <left style="thin">
         <color rgb="FFFFFFFF"/>
       </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
       <right style="thin">
         <color rgb="FFFFFFFF"/>
       </right>
@@ -1035,7 +1000,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="113">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1120,19 +1085,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="5" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="18" fillId="5" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="10" fillId="5" borderId="4" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="18" fillId="5" borderId="4" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="5" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="18" fillId="5" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1144,7 +1109,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="20" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1152,311 +1117,299 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="18" fillId="6" borderId="7" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="6" borderId="8" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="18" fillId="6" borderId="10" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="6" borderId="11" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="18" fillId="6" borderId="12" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="7" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="7" borderId="13" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="2" borderId="15" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="13" fillId="7" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="24" fillId="9" borderId="16" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="26" fillId="9" borderId="17" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="14" fillId="2" borderId="18" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="24" fillId="9" borderId="18" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="27" fillId="9" borderId="17" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="2" borderId="18" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="2" borderId="17" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="2" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="2" borderId="21" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="14" fillId="2" borderId="20" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="2" borderId="22" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="14" fillId="2" borderId="20" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="7" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="2" borderId="23" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="26" fillId="9" borderId="16" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="2" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="2" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="28" fillId="2" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="36" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="36" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="12" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="12" fillId="2" borderId="27" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="12" borderId="27" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="12" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="14" fillId="2" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="9" borderId="27" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="9" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="10" fillId="6" borderId="7" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="6" borderId="8" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="6" borderId="6" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="10" fillId="6" borderId="10" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="6" borderId="11" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="6" borderId="10" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="10" fillId="6" borderId="12" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="24" fillId="6" borderId="13" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="7" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="7" borderId="14" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="28" fillId="2" borderId="16" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="13" fillId="7" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="9" borderId="17" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="29" fillId="9" borderId="18" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="14" fillId="2" borderId="19" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="27" fillId="9" borderId="19" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="2" borderId="19" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="2" borderId="18" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="2" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="28" fillId="2" borderId="22" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="14" fillId="2" borderId="21" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="2" borderId="23" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="14" fillId="2" borderId="21" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="7" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="28" fillId="2" borderId="24" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="27" fillId="9" borderId="17" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="29" fillId="9" borderId="17" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="2" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="28" fillId="2" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="30" fillId="2" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="34" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="39" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="39" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="12" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="2" borderId="28" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="13" fillId="12" borderId="28" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="13" fillId="12" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="9" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="14" fillId="2" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="13" fillId="9" borderId="28" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="13" fillId="9" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="40" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="172" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1468,35 +1421,35 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="8" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="38" fillId="8" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="13" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="29" fillId="13" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="42" fillId="14" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="39" fillId="14" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="33" fillId="0" borderId="31" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="26" fillId="0" borderId="30" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="31" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="30" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="15" borderId="31" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="0" fillId="15" borderId="30" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1632,8 +1585,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>145440</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>210960</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>211680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1643,7 +1596,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="142560" y="2262600"/>
-          <a:ext cx="2880" cy="3749400"/>
+          <a:ext cx="2880" cy="5474160"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1674,14 +1627,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>135720</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>216000</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>216720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>305640</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>216000</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>216720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1690,7 +1643,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="135720" y="3423960"/>
+          <a:off x="135720" y="3748320"/>
           <a:ext cx="169920" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1723,14 +1676,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>135720</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>217800</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>219600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>305640</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>217800</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>219600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1739,7 +1692,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="135720" y="6018840"/>
+          <a:off x="135720" y="7744680"/>
           <a:ext cx="169920" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1772,14 +1725,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>135720</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>216000</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>216720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>305640</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>216000</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>216720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1788,7 +1741,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="135720" y="3423960"/>
+          <a:off x="135720" y="3748320"/>
           <a:ext cx="169920" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1831,9 +1784,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>178560</xdr:colOff>
+      <xdr:colOff>177120</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>92520</xdr:rowOff>
+      <xdr:rowOff>91080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1843,7 +1796,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6514920" y="6991200"/>
-          <a:ext cx="178560" cy="1102320"/>
+          <a:ext cx="177120" cy="1100880"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1893,9 +1846,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>48600</xdr:colOff>
+      <xdr:colOff>47160</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>149760</xdr:rowOff>
+      <xdr:rowOff>148320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1905,7 +1858,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="3809880"/>
-          <a:ext cx="492840" cy="149760"/>
+          <a:ext cx="491400" cy="148320"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1956,8 +1909,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2127,29 +2080,29 @@
       <c r="H9" s="33"/>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
       <c r="N9" s="30"/>
       <c r="O9" s="31"/>
       <c r="P9" s="30"/>
       <c r="Q9" s="30"/>
     </row>
     <row r="10" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
       <c r="N10" s="30"/>
       <c r="O10" s="31"/>
       <c r="P10" s="30"/>
@@ -2164,577 +2117,662 @@
       <c r="E11" s="32"/>
       <c r="F11" s="32"/>
       <c r="G11" s="32"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
       <c r="N11" s="30"/>
       <c r="O11" s="31"/>
       <c r="P11" s="30"/>
       <c r="Q11" s="30"/>
     </row>
-    <row r="12" customFormat="false" ht="5.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
       <c r="N12" s="30"/>
       <c r="O12" s="31"/>
       <c r="P12" s="30"/>
       <c r="Q12" s="30"/>
     </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="42"/>
+    <row r="13" customFormat="false" ht="5.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="N13" s="30"/>
       <c r="O13" s="31"/>
       <c r="P13" s="30"/>
       <c r="Q13" s="30"/>
     </row>
-    <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="43" t="s">
+    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="L14" s="45"/>
-      <c r="M14" s="45" t="s">
-        <v>19</v>
-      </c>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
       <c r="N14" s="30"/>
       <c r="O14" s="31"/>
       <c r="P14" s="30"/>
       <c r="Q14" s="30"/>
     </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="46"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="49" t="n">
-        <f aca="false">SUM(H15:H24)</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="50"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="52"/>
+    <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="42"/>
+      <c r="M15" s="42" t="s">
+        <v>20</v>
+      </c>
       <c r="N15" s="30"/>
       <c r="O15" s="31"/>
       <c r="P15" s="30"/>
       <c r="Q15" s="30"/>
     </row>
     <row r="16" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="53"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="52"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="46" t="n">
+        <f aca="false">SUM(H16:H27)</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="47"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="49"/>
       <c r="N16" s="30"/>
       <c r="O16" s="31"/>
       <c r="P16" s="30"/>
       <c r="Q16" s="30"/>
     </row>
     <row r="17" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="53"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="52"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="49"/>
       <c r="N17" s="30"/>
       <c r="O17" s="31"/>
       <c r="P17" s="30"/>
       <c r="Q17" s="30"/>
     </row>
     <row r="18" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="53"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="51"/>
-      <c r="M18" s="52"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="49"/>
       <c r="N18" s="30"/>
       <c r="O18" s="31"/>
       <c r="P18" s="30"/>
       <c r="Q18" s="30"/>
     </row>
     <row r="19" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="53"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="52"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="49"/>
       <c r="N19" s="30"/>
       <c r="O19" s="31"/>
       <c r="P19" s="30"/>
       <c r="Q19" s="30"/>
     </row>
-    <row r="20" customFormat="false" ht="30" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="53" t="str">
-        <f aca="false">IF(C20&lt;&gt;"",B19+1,"")</f>
-        <v/>
-      </c>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="54"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="52"/>
+    <row r="20" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="50"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="49"/>
       <c r="N20" s="30"/>
       <c r="O20" s="31"/>
       <c r="P20" s="30"/>
       <c r="Q20" s="30"/>
     </row>
-    <row r="21" customFormat="false" ht="30" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="53" t="str">
-        <f aca="false">IF(C21&lt;&gt;"",B20+1,"")</f>
-        <v/>
-      </c>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="56"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="57"/>
-      <c r="M21" s="52"/>
+    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B21" s="50"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="49"/>
       <c r="N21" s="30"/>
       <c r="O21" s="31"/>
       <c r="P21" s="30"/>
       <c r="Q21" s="30"/>
     </row>
-    <row r="22" customFormat="false" ht="30" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="53" t="str">
-        <f aca="false">IF(C22&lt;&gt;"",B21+1,"")</f>
-        <v/>
-      </c>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="57"/>
-      <c r="L22" s="57"/>
-      <c r="M22" s="52"/>
+    <row r="22" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B22" s="50"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="49"/>
       <c r="N22" s="30"/>
       <c r="O22" s="31"/>
       <c r="P22" s="30"/>
       <c r="Q22" s="30"/>
     </row>
     <row r="23" customFormat="false" ht="30" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="53" t="str">
+      <c r="B23" s="50" t="str">
         <f aca="false">IF(C23&lt;&gt;"",B22+1,"")</f>
         <v/>
       </c>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="57"/>
-      <c r="L23" s="57"/>
-      <c r="M23" s="52"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="49"/>
       <c r="N23" s="30"/>
       <c r="O23" s="31"/>
       <c r="P23" s="30"/>
       <c r="Q23" s="30"/>
     </row>
     <row r="24" customFormat="false" ht="30" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="58" t="str">
+      <c r="B24" s="50" t="str">
         <f aca="false">IF(C24&lt;&gt;"",B23+1,"")</f>
         <v/>
       </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="62"/>
-      <c r="L24" s="62"/>
-      <c r="M24" s="63"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="55"/>
+      <c r="M24" s="49"/>
       <c r="N24" s="30"/>
       <c r="O24" s="31"/>
       <c r="P24" s="30"/>
       <c r="Q24" s="30"/>
     </row>
-    <row r="25" customFormat="false" ht="5.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="30" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="50" t="str">
+        <f aca="false">IF(C25&lt;&gt;"",B24+1,"")</f>
+        <v/>
+      </c>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="55"/>
+      <c r="M25" s="49"/>
       <c r="N25" s="30"/>
       <c r="O25" s="31"/>
       <c r="P25" s="30"/>
       <c r="Q25" s="30"/>
     </row>
-    <row r="26" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="64"/>
-      <c r="J26" s="64"/>
-      <c r="K26" s="64"/>
-      <c r="L26" s="64"/>
-      <c r="M26" s="64"/>
+    <row r="26" customFormat="false" ht="30" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B26" s="50" t="str">
+        <f aca="false">IF(C26&lt;&gt;"",B25+1,"")</f>
+        <v/>
+      </c>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="55"/>
+      <c r="M26" s="49"/>
       <c r="N26" s="30"/>
       <c r="O26" s="31"/>
       <c r="P26" s="30"/>
       <c r="Q26" s="30"/>
     </row>
-    <row r="27" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="65" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="65"/>
-      <c r="F27" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="45"/>
-      <c r="J27" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="K27" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="L27" s="45"/>
-      <c r="M27" s="45" t="s">
-        <v>19</v>
-      </c>
+    <row r="27" customFormat="false" ht="30" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="56" t="str">
+        <f aca="false">IF(C27&lt;&gt;"",B26+1,"")</f>
+        <v/>
+      </c>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="59"/>
+      <c r="K27" s="60"/>
+      <c r="L27" s="60"/>
+      <c r="M27" s="61"/>
       <c r="N27" s="30"/>
       <c r="O27" s="31"/>
       <c r="P27" s="30"/>
       <c r="Q27" s="30"/>
     </row>
-    <row r="28" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="46"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="49" t="n">
-        <f aca="false">SUM(H28:H32)</f>
-        <v>0</v>
-      </c>
-      <c r="J28" s="67"/>
-      <c r="K28" s="68"/>
-      <c r="L28" s="68"/>
-      <c r="M28" s="52"/>
+    <row r="28" customFormat="false" ht="5.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="N28" s="30"/>
       <c r="O28" s="31"/>
       <c r="P28" s="30"/>
       <c r="Q28" s="30"/>
     </row>
-    <row r="29" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="53"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="67"/>
-      <c r="K29" s="68"/>
-      <c r="L29" s="68"/>
-      <c r="M29" s="52"/>
+    <row r="29" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="62"/>
+      <c r="K29" s="62"/>
+      <c r="L29" s="62"/>
+      <c r="M29" s="62"/>
       <c r="N29" s="30"/>
       <c r="O29" s="31"/>
       <c r="P29" s="30"/>
       <c r="Q29" s="30"/>
     </row>
-    <row r="30" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="53"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="67"/>
-      <c r="K30" s="68"/>
-      <c r="L30" s="68"/>
-      <c r="M30" s="52"/>
+    <row r="30" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="40"/>
+      <c r="D30" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="63"/>
+      <c r="F30" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="K30" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42" t="s">
+        <v>20</v>
+      </c>
       <c r="N30" s="30"/>
       <c r="O30" s="31"/>
       <c r="P30" s="30"/>
       <c r="Q30" s="30"/>
     </row>
-    <row r="31" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="53"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="67"/>
-      <c r="K31" s="68"/>
-      <c r="L31" s="68"/>
-      <c r="M31" s="52"/>
+    <row r="31" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="43"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="64"/>
+      <c r="I31" s="46" t="n">
+        <f aca="false">SUM(H31:H37)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="47"/>
+      <c r="K31" s="65"/>
+      <c r="L31" s="65"/>
+      <c r="M31" s="49"/>
       <c r="N31" s="30"/>
       <c r="O31" s="31"/>
       <c r="P31" s="30"/>
       <c r="Q31" s="30"/>
     </row>
-    <row r="32" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="53"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="55"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="67"/>
-      <c r="K32" s="68"/>
-      <c r="L32" s="68"/>
-      <c r="M32" s="52"/>
+    <row r="32" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="50"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="65"/>
+      <c r="L32" s="65"/>
+      <c r="M32" s="49"/>
       <c r="N32" s="30"/>
       <c r="O32" s="31"/>
       <c r="P32" s="30"/>
       <c r="Q32" s="30"/>
     </row>
-    <row r="33" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="30"/>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="70" t="s">
-        <v>22</v>
-      </c>
-      <c r="H33" s="71" t="n">
-        <f aca="false">I28+I15</f>
-        <v>0</v>
-      </c>
-      <c r="I33" s="69"/>
-      <c r="J33" s="69"/>
-      <c r="K33" s="69"/>
-      <c r="L33" s="69"/>
-      <c r="M33" s="69"/>
+    <row r="33" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B33" s="50"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="52"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="65"/>
+      <c r="L33" s="65"/>
+      <c r="M33" s="49"/>
       <c r="N33" s="30"/>
       <c r="O33" s="31"/>
       <c r="P33" s="30"/>
       <c r="Q33" s="30"/>
     </row>
-    <row r="34" customFormat="false" ht="5.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="72"/>
-      <c r="G34" s="72"/>
-      <c r="H34" s="72"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="72"/>
-      <c r="K34" s="72"/>
-      <c r="L34" s="72"/>
-      <c r="M34" s="72"/>
+    <row r="34" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B34" s="50"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="47"/>
+      <c r="K34" s="65"/>
+      <c r="L34" s="65"/>
+      <c r="M34" s="49"/>
       <c r="N34" s="30"/>
       <c r="O34" s="31"/>
       <c r="P34" s="30"/>
       <c r="Q34" s="30"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="73" t="s">
+    <row r="35" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B35" s="50"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="65"/>
+      <c r="L35" s="65"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="30"/>
+      <c r="O35" s="31"/>
+      <c r="P35" s="30"/>
+      <c r="Q35" s="30"/>
+    </row>
+    <row r="36" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B36" s="50"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="47"/>
+      <c r="K36" s="65"/>
+      <c r="L36" s="65"/>
+      <c r="M36" s="49"/>
+      <c r="N36" s="30"/>
+      <c r="O36" s="31"/>
+      <c r="P36" s="30"/>
+      <c r="Q36" s="30"/>
+    </row>
+    <row r="37" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B37" s="50"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="47"/>
+      <c r="K37" s="65"/>
+      <c r="L37" s="65"/>
+      <c r="M37" s="49"/>
+      <c r="N37" s="30"/>
+      <c r="O37" s="31"/>
+      <c r="P37" s="30"/>
+      <c r="Q37" s="30"/>
+    </row>
+    <row r="38" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="30"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="66"/>
+      <c r="G38" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="73"/>
-      <c r="D35" s="73"/>
-      <c r="E35" s="73"/>
-      <c r="F35" s="73"/>
-      <c r="G35" s="73"/>
-      <c r="H35" s="73"/>
-      <c r="I35" s="73"/>
-      <c r="J35" s="73"/>
-      <c r="K35" s="73"/>
-      <c r="L35" s="73"/>
-      <c r="M35" s="73"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="74"/>
-      <c r="C36" s="74"/>
-      <c r="D36" s="74"/>
-      <c r="E36" s="74"/>
-      <c r="F36" s="74"/>
-      <c r="G36" s="74"/>
-      <c r="H36" s="74"/>
-      <c r="I36" s="74"/>
-      <c r="J36" s="74"/>
-      <c r="K36" s="74"/>
-      <c r="L36" s="74"/>
-      <c r="M36" s="74"/>
-    </row>
-    <row r="37" s="75" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="76"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="78"/>
-      <c r="G37" s="78"/>
-      <c r="H37" s="78"/>
-      <c r="I37" s="78"/>
-      <c r="J37" s="79"/>
-      <c r="K37" s="79"/>
-      <c r="L37" s="79"/>
-      <c r="M37" s="79"/>
-      <c r="O37" s="80"/>
-    </row>
-    <row r="38" s="75" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="76"/>
-      <c r="C38" s="76"/>
-      <c r="D38" s="76"/>
-      <c r="E38" s="76"/>
-      <c r="F38" s="81" t="s">
+      <c r="H38" s="68" t="n">
+        <f aca="false">I31+I16</f>
+        <v>0</v>
+      </c>
+      <c r="I38" s="66"/>
+      <c r="J38" s="66"/>
+      <c r="K38" s="66"/>
+      <c r="L38" s="66"/>
+      <c r="M38" s="66"/>
+      <c r="N38" s="30"/>
+      <c r="O38" s="31"/>
+      <c r="P38" s="30"/>
+      <c r="Q38" s="30"/>
+    </row>
+    <row r="39" customFormat="false" ht="5.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="69"/>
+      <c r="I39" s="69"/>
+      <c r="J39" s="69"/>
+      <c r="K39" s="69"/>
+      <c r="L39" s="69"/>
+      <c r="M39" s="69"/>
+      <c r="N39" s="30"/>
+      <c r="O39" s="31"/>
+      <c r="P39" s="30"/>
+      <c r="Q39" s="30"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B40" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="G38" s="81"/>
-      <c r="H38" s="79"/>
-      <c r="I38" s="79"/>
-      <c r="J38" s="81" t="s">
+      <c r="C40" s="70"/>
+      <c r="D40" s="70"/>
+      <c r="E40" s="70"/>
+      <c r="F40" s="70"/>
+      <c r="G40" s="70"/>
+      <c r="H40" s="70"/>
+      <c r="I40" s="70"/>
+      <c r="J40" s="70"/>
+      <c r="K40" s="70"/>
+      <c r="L40" s="70"/>
+      <c r="M40" s="70"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="71"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="71"/>
+      <c r="F41" s="71"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="71"/>
+      <c r="I41" s="71"/>
+      <c r="J41" s="71"/>
+      <c r="K41" s="71"/>
+      <c r="L41" s="71"/>
+      <c r="M41" s="71"/>
+    </row>
+    <row r="42" s="72" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B42" s="73"/>
+      <c r="C42" s="73"/>
+      <c r="D42" s="73"/>
+      <c r="E42" s="74"/>
+      <c r="F42" s="75"/>
+      <c r="G42" s="75"/>
+      <c r="H42" s="75"/>
+      <c r="I42" s="75"/>
+      <c r="J42" s="76"/>
+      <c r="K42" s="76"/>
+      <c r="L42" s="76"/>
+      <c r="M42" s="76"/>
+      <c r="O42" s="77"/>
+    </row>
+    <row r="43" s="72" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B43" s="73"/>
+      <c r="C43" s="73"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="K38" s="81"/>
-      <c r="L38" s="81"/>
-      <c r="M38" s="81"/>
-      <c r="O38" s="80"/>
-    </row>
-    <row r="39" s="75" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="76"/>
-      <c r="C39" s="76"/>
-      <c r="D39" s="76"/>
-      <c r="E39" s="82"/>
-      <c r="F39" s="76"/>
-      <c r="G39" s="76"/>
-      <c r="H39" s="76"/>
-      <c r="I39" s="76"/>
-      <c r="J39" s="78"/>
-      <c r="K39" s="78"/>
-      <c r="L39" s="78"/>
-      <c r="M39" s="78"/>
-      <c r="O39" s="80"/>
-    </row>
-    <row r="40" s="75" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="83" t="s">
+      <c r="G43" s="78"/>
+      <c r="H43" s="76"/>
+      <c r="I43" s="76"/>
+      <c r="J43" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="83"/>
-      <c r="D40" s="84"/>
-      <c r="E40" s="85"/>
-      <c r="F40" s="86"/>
-      <c r="G40" s="86"/>
-      <c r="H40" s="86"/>
-      <c r="I40" s="86"/>
-      <c r="J40" s="86"/>
-      <c r="K40" s="86"/>
-      <c r="L40" s="86"/>
-      <c r="M40" s="86"/>
-      <c r="O40" s="80"/>
-    </row>
-    <row r="41" s="75" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="87" t="str">
+      <c r="K43" s="78"/>
+      <c r="L43" s="78"/>
+      <c r="M43" s="78"/>
+      <c r="O43" s="77"/>
+    </row>
+    <row r="44" s="72" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B44" s="73"/>
+      <c r="C44" s="73"/>
+      <c r="D44" s="73"/>
+      <c r="E44" s="79"/>
+      <c r="F44" s="73"/>
+      <c r="G44" s="73"/>
+      <c r="H44" s="73"/>
+      <c r="I44" s="73"/>
+      <c r="J44" s="75"/>
+      <c r="K44" s="75"/>
+      <c r="L44" s="75"/>
+      <c r="M44" s="75"/>
+      <c r="O44" s="77"/>
+    </row>
+    <row r="45" s="72" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B45" s="80"/>
+      <c r="C45" s="80"/>
+      <c r="D45" s="81"/>
+      <c r="E45" s="82"/>
+      <c r="F45" s="83"/>
+      <c r="G45" s="83"/>
+      <c r="H45" s="83"/>
+      <c r="I45" s="83"/>
+      <c r="J45" s="83"/>
+      <c r="K45" s="83"/>
+      <c r="L45" s="83"/>
+      <c r="M45" s="83"/>
+      <c r="O45" s="77"/>
+    </row>
+    <row r="46" s="72" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B46" s="84" t="str">
         <f aca="true">CELL("FILENAME")</f>
-        <v>'file:///opt/plr/templates/TEMPLATE.xlsx'#$FOLHA METAS</v>
-      </c>
-      <c r="C41" s="88"/>
-      <c r="E41" s="89"/>
-      <c r="O41" s="80"/>
-    </row>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>'file:///opt/plr/templates/TEMPLATE_METAS.xlsx'#$FOLHA METAS</v>
+      </c>
+      <c r="C46" s="85"/>
+      <c r="E46" s="86"/>
+      <c r="O46" s="77"/>
+    </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2744,7 +2782,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="75">
+  <mergeCells count="78">
     <mergeCell ref="D1:K2"/>
     <mergeCell ref="L1:M2"/>
     <mergeCell ref="B3:M3"/>
@@ -2755,25 +2793,21 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="I7:M7"/>
     <mergeCell ref="B9:G9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="I9:M9"/>
     <mergeCell ref="B10:G10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="I10:M10"/>
     <mergeCell ref="B11:G11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="B14:M14"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="F15:G15"/>
-    <mergeCell ref="I15:I24"/>
+    <mergeCell ref="H15:I15"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="F16:G16"/>
+    <mergeCell ref="I16:I27"/>
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="F17:G17"/>
@@ -2784,42 +2818,49 @@
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="K19:L19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="K22:L22"/>
     <mergeCell ref="C23:G23"/>
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="C24:G24"/>
     <mergeCell ref="K24:L24"/>
-    <mergeCell ref="B26:M26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="C27:G27"/>
     <mergeCell ref="K27:L27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="I28:I32"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="B29:M29"/>
+    <mergeCell ref="D30:E30"/>
     <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
     <mergeCell ref="K30:L30"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="F31:G31"/>
+    <mergeCell ref="I31:I37"/>
     <mergeCell ref="K31:L31"/>
     <mergeCell ref="C32:E32"/>
     <mergeCell ref="F32:G32"/>
     <mergeCell ref="K32:L32"/>
-    <mergeCell ref="F34:M34"/>
-    <mergeCell ref="B35:M35"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="F39:M39"/>
+    <mergeCell ref="B40:M40"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="J43:M43"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
   <pageMargins left="0.118055555555556" right="0.118055555555556" top="0.196527777777778" bottom="0.196527777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2848,216 +2889,216 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="90" width="1.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="90" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="90" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="90" width="1.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="90" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="90" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="90" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="87" width="1.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="87" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="87" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="87" width="1.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="87" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="87" width="13.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="87" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="91" t="e">
+      <c r="B1" s="88" t="e">
         <f aca="false">#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="C1" s="92" t="n">
-        <f aca="false">'FOLHA METAS'!C21:G21</f>
+      <c r="C1" s="89" t="n">
+        <f aca="false">'FOLHA METAS'!C24:G24</f>
         <v>0</v>
       </c>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="93" t="s">
+      <c r="E2" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="93" t="s">
+      <c r="F2" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="93" t="s">
+      <c r="G2" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="93" t="s">
+      <c r="H2" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="93" t="s">
+      <c r="I2" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="93" t="s">
+      <c r="J2" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="93" t="s">
+      <c r="K2" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="93" t="s">
+      <c r="L2" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="93" t="s">
+      <c r="M2" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="93" t="s">
+      <c r="N2" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="94"/>
-      <c r="P2" s="93" t="s">
+      <c r="O2" s="91"/>
+      <c r="P2" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="93" t="s">
+      <c r="Q2" s="90" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="98" t="n">
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="94"/>
+      <c r="P3" s="95" t="n">
         <f aca="false">SUM(C3:N3)</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="99" t="n">
+      <c r="Q3" s="96" t="n">
         <f aca="false">IFERROR(AVERAGE(C3:N3),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="96"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="101"/>
-      <c r="P4" s="102" t="n">
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="98"/>
+      <c r="P4" s="99" t="n">
         <f aca="false">SUM(C4:N4)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="103" t="n">
+      <c r="Q4" s="100" t="n">
         <f aca="false">IFERROR(AVERAGE(C4:N4),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H5" s="104"/>
-      <c r="I5" s="105"/>
-      <c r="J5" s="105"/>
-      <c r="K5" s="105"/>
-      <c r="L5" s="105"/>
-      <c r="M5" s="105"/>
-      <c r="N5" s="105"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="107"/>
-      <c r="S5" s="107"/>
-      <c r="T5" s="107"/>
-      <c r="U5" s="107"/>
-      <c r="V5" s="107"/>
-      <c r="W5" s="107"/>
-      <c r="X5" s="107"/>
-      <c r="Y5" s="107"/>
-      <c r="Z5" s="107"/>
-      <c r="AA5" s="107"/>
-      <c r="AB5" s="107"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="102"/>
+      <c r="K5" s="102"/>
+      <c r="L5" s="102"/>
+      <c r="M5" s="102"/>
+      <c r="N5" s="102"/>
+      <c r="O5" s="103"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="103"/>
+      <c r="R5" s="104"/>
+      <c r="S5" s="104"/>
+      <c r="T5" s="104"/>
+      <c r="U5" s="104"/>
+      <c r="V5" s="104"/>
+      <c r="W5" s="104"/>
+      <c r="X5" s="104"/>
+      <c r="Y5" s="104"/>
+      <c r="Z5" s="104"/>
+      <c r="AA5" s="104"/>
+      <c r="AB5" s="104"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H6" s="104"/>
-      <c r="I6" s="105"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="105"/>
-      <c r="M6" s="105"/>
-      <c r="N6" s="105"/>
-      <c r="O6" s="106"/>
-      <c r="P6" s="106"/>
-      <c r="Q6" s="106"/>
-      <c r="R6" s="107"/>
-      <c r="S6" s="107"/>
-      <c r="T6" s="107"/>
-      <c r="U6" s="107"/>
-      <c r="V6" s="107"/>
-      <c r="W6" s="107"/>
-      <c r="X6" s="107"/>
-      <c r="Y6" s="107"/>
-      <c r="Z6" s="107"/>
-      <c r="AA6" s="107"/>
-      <c r="AB6" s="107"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="102"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="102"/>
+      <c r="M6" s="102"/>
+      <c r="N6" s="102"/>
+      <c r="O6" s="103"/>
+      <c r="P6" s="103"/>
+      <c r="Q6" s="103"/>
+      <c r="R6" s="104"/>
+      <c r="S6" s="104"/>
+      <c r="T6" s="104"/>
+      <c r="U6" s="104"/>
+      <c r="V6" s="104"/>
+      <c r="W6" s="104"/>
+      <c r="X6" s="104"/>
+      <c r="Y6" s="104"/>
+      <c r="Z6" s="104"/>
+      <c r="AA6" s="104"/>
+      <c r="AB6" s="104"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="108" t="e">
+      <c r="B7" s="105" t="e">
         <f aca="false">B1</f>
         <v>#REF!</v>
       </c>
-      <c r="C7" s="109" t="e">
+      <c r="C7" s="106" t="e">
         <f aca="false">#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D7" s="109"/>
-      <c r="E7" s="109"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="109"/>
-      <c r="J7" s="109"/>
-      <c r="K7" s="109"/>
-      <c r="L7" s="109"/>
-      <c r="M7" s="109"/>
-      <c r="N7" s="109"/>
-      <c r="O7" s="110"/>
-      <c r="P7" s="110"/>
-      <c r="Q7" s="106"/>
-      <c r="R7" s="107"/>
-      <c r="S7" s="107"/>
-      <c r="T7" s="107"/>
-      <c r="U7" s="107"/>
-      <c r="V7" s="107"/>
-      <c r="W7" s="107"/>
-      <c r="X7" s="107"/>
-      <c r="Y7" s="107"/>
-      <c r="Z7" s="107"/>
-      <c r="AA7" s="107"/>
-      <c r="AB7" s="107"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="106"/>
+      <c r="F7" s="106"/>
+      <c r="G7" s="106"/>
+      <c r="H7" s="106"/>
+      <c r="I7" s="106"/>
+      <c r="J7" s="106"/>
+      <c r="K7" s="106"/>
+      <c r="L7" s="106"/>
+      <c r="M7" s="106"/>
+      <c r="N7" s="106"/>
+      <c r="O7" s="107"/>
+      <c r="P7" s="107"/>
+      <c r="Q7" s="103"/>
+      <c r="R7" s="104"/>
+      <c r="S7" s="104"/>
+      <c r="T7" s="104"/>
+      <c r="U7" s="104"/>
+      <c r="V7" s="104"/>
+      <c r="W7" s="104"/>
+      <c r="X7" s="104"/>
+      <c r="Y7" s="104"/>
+      <c r="Z7" s="104"/>
+      <c r="AA7" s="104"/>
+      <c r="AB7" s="104"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -3088,216 +3129,216 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="90" width="1.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="90" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="90" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="90" width="1.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="90" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="90" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="90" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="87" width="1.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="87" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="87" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="87" width="1.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="87" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="87" width="13.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="87" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="91" t="e">
+      <c r="B1" s="88" t="e">
         <f aca="false">#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="C1" s="92" t="n">
-        <f aca="false">'FOLHA METAS'!C22:G22</f>
+      <c r="C1" s="89" t="n">
+        <f aca="false">'FOLHA METAS'!C25:G25</f>
         <v>0</v>
       </c>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="93" t="s">
+      <c r="E2" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="93" t="s">
+      <c r="F2" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="93" t="s">
+      <c r="G2" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="93" t="s">
+      <c r="H2" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="93" t="s">
+      <c r="I2" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="93" t="s">
+      <c r="J2" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="93" t="s">
+      <c r="K2" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="93" t="s">
+      <c r="L2" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="93" t="s">
+      <c r="M2" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="93" t="s">
+      <c r="N2" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="94"/>
-      <c r="P2" s="93" t="s">
+      <c r="O2" s="91"/>
+      <c r="P2" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="93" t="s">
+      <c r="Q2" s="90" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="98" t="n">
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="94"/>
+      <c r="P3" s="95" t="n">
         <f aca="false">SUM(C3:N3)</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="99" t="n">
+      <c r="Q3" s="96" t="n">
         <f aca="false">IFERROR(AVERAGE(C3:N3),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="96"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="101"/>
-      <c r="P4" s="102" t="n">
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="98"/>
+      <c r="P4" s="99" t="n">
         <f aca="false">SUM(C4:N4)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="103" t="n">
+      <c r="Q4" s="100" t="n">
         <f aca="false">IFERROR(AVERAGE(C4:N4),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H5" s="104"/>
-      <c r="I5" s="105"/>
-      <c r="J5" s="105"/>
-      <c r="K5" s="105"/>
-      <c r="L5" s="105"/>
-      <c r="M5" s="105"/>
-      <c r="N5" s="105"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="107"/>
-      <c r="S5" s="107"/>
-      <c r="T5" s="107"/>
-      <c r="U5" s="107"/>
-      <c r="V5" s="107"/>
-      <c r="W5" s="107"/>
-      <c r="X5" s="107"/>
-      <c r="Y5" s="107"/>
-      <c r="Z5" s="107"/>
-      <c r="AA5" s="107"/>
-      <c r="AB5" s="107"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="102"/>
+      <c r="K5" s="102"/>
+      <c r="L5" s="102"/>
+      <c r="M5" s="102"/>
+      <c r="N5" s="102"/>
+      <c r="O5" s="103"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="103"/>
+      <c r="R5" s="104"/>
+      <c r="S5" s="104"/>
+      <c r="T5" s="104"/>
+      <c r="U5" s="104"/>
+      <c r="V5" s="104"/>
+      <c r="W5" s="104"/>
+      <c r="X5" s="104"/>
+      <c r="Y5" s="104"/>
+      <c r="Z5" s="104"/>
+      <c r="AA5" s="104"/>
+      <c r="AB5" s="104"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H6" s="104"/>
-      <c r="I6" s="105"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="105"/>
-      <c r="M6" s="105"/>
-      <c r="N6" s="105"/>
-      <c r="O6" s="106"/>
-      <c r="P6" s="106"/>
-      <c r="Q6" s="106"/>
-      <c r="R6" s="107"/>
-      <c r="S6" s="107"/>
-      <c r="T6" s="107"/>
-      <c r="U6" s="107"/>
-      <c r="V6" s="107"/>
-      <c r="W6" s="107"/>
-      <c r="X6" s="107"/>
-      <c r="Y6" s="107"/>
-      <c r="Z6" s="107"/>
-      <c r="AA6" s="107"/>
-      <c r="AB6" s="107"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="102"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="102"/>
+      <c r="M6" s="102"/>
+      <c r="N6" s="102"/>
+      <c r="O6" s="103"/>
+      <c r="P6" s="103"/>
+      <c r="Q6" s="103"/>
+      <c r="R6" s="104"/>
+      <c r="S6" s="104"/>
+      <c r="T6" s="104"/>
+      <c r="U6" s="104"/>
+      <c r="V6" s="104"/>
+      <c r="W6" s="104"/>
+      <c r="X6" s="104"/>
+      <c r="Y6" s="104"/>
+      <c r="Z6" s="104"/>
+      <c r="AA6" s="104"/>
+      <c r="AB6" s="104"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="108" t="e">
+      <c r="B7" s="105" t="e">
         <f aca="false">B1</f>
         <v>#REF!</v>
       </c>
-      <c r="C7" s="109" t="e">
+      <c r="C7" s="106" t="e">
         <f aca="false">#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D7" s="109"/>
-      <c r="E7" s="109"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="109"/>
-      <c r="J7" s="109"/>
-      <c r="K7" s="109"/>
-      <c r="L7" s="109"/>
-      <c r="M7" s="109"/>
-      <c r="N7" s="109"/>
-      <c r="O7" s="110"/>
-      <c r="P7" s="110"/>
-      <c r="Q7" s="106"/>
-      <c r="R7" s="107"/>
-      <c r="S7" s="107"/>
-      <c r="T7" s="107"/>
-      <c r="U7" s="107"/>
-      <c r="V7" s="107"/>
-      <c r="W7" s="107"/>
-      <c r="X7" s="107"/>
-      <c r="Y7" s="107"/>
-      <c r="Z7" s="107"/>
-      <c r="AA7" s="107"/>
-      <c r="AB7" s="107"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="106"/>
+      <c r="F7" s="106"/>
+      <c r="G7" s="106"/>
+      <c r="H7" s="106"/>
+      <c r="I7" s="106"/>
+      <c r="J7" s="106"/>
+      <c r="K7" s="106"/>
+      <c r="L7" s="106"/>
+      <c r="M7" s="106"/>
+      <c r="N7" s="106"/>
+      <c r="O7" s="107"/>
+      <c r="P7" s="107"/>
+      <c r="Q7" s="103"/>
+      <c r="R7" s="104"/>
+      <c r="S7" s="104"/>
+      <c r="T7" s="104"/>
+      <c r="U7" s="104"/>
+      <c r="V7" s="104"/>
+      <c r="W7" s="104"/>
+      <c r="X7" s="104"/>
+      <c r="Y7" s="104"/>
+      <c r="Z7" s="104"/>
+      <c r="AA7" s="104"/>
+      <c r="AB7" s="104"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -3328,220 +3369,220 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="90" width="1.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="90" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="90" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="90" width="1.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="90" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="90" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="90" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="87" width="1.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="87" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="87" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="87" width="1.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="87" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="87" width="13.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="87" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="91" t="e">
+      <c r="B1" s="88" t="e">
         <f aca="false">#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="C1" s="92" t="n">
-        <f aca="false">'FOLHA METAS'!C15:G15</f>
+      <c r="C1" s="89" t="n">
+        <f aca="false">'FOLHA METAS'!C16:G16</f>
         <v>0</v>
       </c>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="90" t="e">
-        <f aca="false">'FOLHA METAS'!C23:G23</f>
+      <c r="B2" s="87" t="e">
+        <f aca="false">'FOLHA METAS'!C26:G26</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="93" t="s">
+      <c r="E2" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="93" t="s">
+      <c r="F2" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="93" t="s">
+      <c r="G2" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="93" t="s">
+      <c r="H2" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="93" t="s">
+      <c r="I2" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="93" t="s">
+      <c r="J2" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="93" t="s">
+      <c r="K2" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="93" t="s">
+      <c r="L2" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="93" t="s">
+      <c r="M2" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="93" t="s">
+      <c r="N2" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="94"/>
-      <c r="P2" s="93" t="s">
+      <c r="O2" s="91"/>
+      <c r="P2" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="93" t="s">
+      <c r="Q2" s="90" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="98" t="n">
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="94"/>
+      <c r="P3" s="95" t="n">
         <f aca="false">SUM(C3:N3)</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="99" t="n">
+      <c r="Q3" s="96" t="n">
         <f aca="false">IFERROR(AVERAGE(C3:N3),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="96"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="101"/>
-      <c r="P4" s="102" t="n">
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="98"/>
+      <c r="P4" s="99" t="n">
         <f aca="false">SUM(C4:N4)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="103" t="n">
+      <c r="Q4" s="100" t="n">
         <f aca="false">IFERROR(AVERAGE(C4:N4),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H5" s="104"/>
-      <c r="I5" s="105"/>
-      <c r="J5" s="105"/>
-      <c r="K5" s="105"/>
-      <c r="L5" s="105"/>
-      <c r="M5" s="105"/>
-      <c r="N5" s="105"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="107"/>
-      <c r="S5" s="107"/>
-      <c r="T5" s="107"/>
-      <c r="U5" s="107"/>
-      <c r="V5" s="107"/>
-      <c r="W5" s="107"/>
-      <c r="X5" s="107"/>
-      <c r="Y5" s="107"/>
-      <c r="Z5" s="107"/>
-      <c r="AA5" s="107"/>
-      <c r="AB5" s="107"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="102"/>
+      <c r="K5" s="102"/>
+      <c r="L5" s="102"/>
+      <c r="M5" s="102"/>
+      <c r="N5" s="102"/>
+      <c r="O5" s="103"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="103"/>
+      <c r="R5" s="104"/>
+      <c r="S5" s="104"/>
+      <c r="T5" s="104"/>
+      <c r="U5" s="104"/>
+      <c r="V5" s="104"/>
+      <c r="W5" s="104"/>
+      <c r="X5" s="104"/>
+      <c r="Y5" s="104"/>
+      <c r="Z5" s="104"/>
+      <c r="AA5" s="104"/>
+      <c r="AB5" s="104"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H6" s="104"/>
-      <c r="I6" s="105"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="105"/>
-      <c r="M6" s="105"/>
-      <c r="N6" s="105"/>
-      <c r="O6" s="106"/>
-      <c r="P6" s="106"/>
-      <c r="Q6" s="106"/>
-      <c r="R6" s="107"/>
-      <c r="S6" s="107"/>
-      <c r="T6" s="107"/>
-      <c r="U6" s="107"/>
-      <c r="V6" s="107"/>
-      <c r="W6" s="107"/>
-      <c r="X6" s="107"/>
-      <c r="Y6" s="107"/>
-      <c r="Z6" s="107"/>
-      <c r="AA6" s="107"/>
-      <c r="AB6" s="107"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="102"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="102"/>
+      <c r="M6" s="102"/>
+      <c r="N6" s="102"/>
+      <c r="O6" s="103"/>
+      <c r="P6" s="103"/>
+      <c r="Q6" s="103"/>
+      <c r="R6" s="104"/>
+      <c r="S6" s="104"/>
+      <c r="T6" s="104"/>
+      <c r="U6" s="104"/>
+      <c r="V6" s="104"/>
+      <c r="W6" s="104"/>
+      <c r="X6" s="104"/>
+      <c r="Y6" s="104"/>
+      <c r="Z6" s="104"/>
+      <c r="AA6" s="104"/>
+      <c r="AB6" s="104"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="108" t="e">
+      <c r="B7" s="105" t="e">
         <f aca="false">B1</f>
         <v>#REF!</v>
       </c>
-      <c r="C7" s="109" t="e">
+      <c r="C7" s="106" t="e">
         <f aca="false">#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D7" s="109"/>
-      <c r="E7" s="109"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="109"/>
-      <c r="J7" s="109"/>
-      <c r="K7" s="109"/>
-      <c r="L7" s="109"/>
-      <c r="M7" s="109"/>
-      <c r="N7" s="109"/>
-      <c r="O7" s="110"/>
-      <c r="P7" s="110"/>
-      <c r="Q7" s="106"/>
-      <c r="R7" s="107"/>
-      <c r="S7" s="107"/>
-      <c r="T7" s="107"/>
-      <c r="U7" s="107"/>
-      <c r="V7" s="107"/>
-      <c r="W7" s="107"/>
-      <c r="X7" s="107"/>
-      <c r="Y7" s="107"/>
-      <c r="Z7" s="107"/>
-      <c r="AA7" s="107"/>
-      <c r="AB7" s="107"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="106"/>
+      <c r="F7" s="106"/>
+      <c r="G7" s="106"/>
+      <c r="H7" s="106"/>
+      <c r="I7" s="106"/>
+      <c r="J7" s="106"/>
+      <c r="K7" s="106"/>
+      <c r="L7" s="106"/>
+      <c r="M7" s="106"/>
+      <c r="N7" s="106"/>
+      <c r="O7" s="107"/>
+      <c r="P7" s="107"/>
+      <c r="Q7" s="103"/>
+      <c r="R7" s="104"/>
+      <c r="S7" s="104"/>
+      <c r="T7" s="104"/>
+      <c r="U7" s="104"/>
+      <c r="V7" s="104"/>
+      <c r="W7" s="104"/>
+      <c r="X7" s="104"/>
+      <c r="Y7" s="104"/>
+      <c r="Z7" s="104"/>
+      <c r="AA7" s="104"/>
+      <c r="AB7" s="104"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -3572,216 +3613,216 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="90" width="1.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="90" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="90" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="90" width="1.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="90" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="90" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="90" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="87" width="1.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="87" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="87" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="87" width="1.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="87" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="87" width="13.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="87" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="91" t="e">
+      <c r="B1" s="88" t="e">
         <f aca="false">#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="C1" s="92" t="n">
-        <f aca="false">'FOLHA METAS'!C24:G24</f>
+      <c r="C1" s="89" t="n">
+        <f aca="false">'FOLHA METAS'!C27:G27</f>
         <v>0</v>
       </c>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="93" t="s">
+      <c r="E2" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="93" t="s">
+      <c r="F2" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="93" t="s">
+      <c r="G2" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="93" t="s">
+      <c r="H2" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="93" t="s">
+      <c r="I2" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="93" t="s">
+      <c r="J2" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="93" t="s">
+      <c r="K2" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="93" t="s">
+      <c r="L2" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="93" t="s">
+      <c r="M2" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="93" t="s">
+      <c r="N2" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="94"/>
-      <c r="P2" s="93" t="s">
+      <c r="O2" s="91"/>
+      <c r="P2" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="93" t="s">
+      <c r="Q2" s="90" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="98" t="n">
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="94"/>
+      <c r="P3" s="95" t="n">
         <f aca="false">SUM(C3:N3)</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="99" t="n">
+      <c r="Q3" s="96" t="n">
         <f aca="false">IFERROR(AVERAGE(C3:N3),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="96"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="101"/>
-      <c r="P4" s="102" t="n">
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="98"/>
+      <c r="P4" s="99" t="n">
         <f aca="false">SUM(C4:N4)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="103" t="n">
+      <c r="Q4" s="100" t="n">
         <f aca="false">IFERROR(AVERAGE(C4:N4),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H5" s="104"/>
-      <c r="I5" s="105"/>
-      <c r="J5" s="105"/>
-      <c r="K5" s="105"/>
-      <c r="L5" s="105"/>
-      <c r="M5" s="105"/>
-      <c r="N5" s="105"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="107"/>
-      <c r="S5" s="107"/>
-      <c r="T5" s="107"/>
-      <c r="U5" s="107"/>
-      <c r="V5" s="107"/>
-      <c r="W5" s="107"/>
-      <c r="X5" s="107"/>
-      <c r="Y5" s="107"/>
-      <c r="Z5" s="107"/>
-      <c r="AA5" s="107"/>
-      <c r="AB5" s="107"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="102"/>
+      <c r="K5" s="102"/>
+      <c r="L5" s="102"/>
+      <c r="M5" s="102"/>
+      <c r="N5" s="102"/>
+      <c r="O5" s="103"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="103"/>
+      <c r="R5" s="104"/>
+      <c r="S5" s="104"/>
+      <c r="T5" s="104"/>
+      <c r="U5" s="104"/>
+      <c r="V5" s="104"/>
+      <c r="W5" s="104"/>
+      <c r="X5" s="104"/>
+      <c r="Y5" s="104"/>
+      <c r="Z5" s="104"/>
+      <c r="AA5" s="104"/>
+      <c r="AB5" s="104"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H6" s="104"/>
-      <c r="I6" s="105"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="105"/>
-      <c r="M6" s="105"/>
-      <c r="N6" s="105"/>
-      <c r="O6" s="106"/>
-      <c r="P6" s="106"/>
-      <c r="Q6" s="106"/>
-      <c r="R6" s="107"/>
-      <c r="S6" s="107"/>
-      <c r="T6" s="107"/>
-      <c r="U6" s="107"/>
-      <c r="V6" s="107"/>
-      <c r="W6" s="107"/>
-      <c r="X6" s="107"/>
-      <c r="Y6" s="107"/>
-      <c r="Z6" s="107"/>
-      <c r="AA6" s="107"/>
-      <c r="AB6" s="107"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="102"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="102"/>
+      <c r="M6" s="102"/>
+      <c r="N6" s="102"/>
+      <c r="O6" s="103"/>
+      <c r="P6" s="103"/>
+      <c r="Q6" s="103"/>
+      <c r="R6" s="104"/>
+      <c r="S6" s="104"/>
+      <c r="T6" s="104"/>
+      <c r="U6" s="104"/>
+      <c r="V6" s="104"/>
+      <c r="W6" s="104"/>
+      <c r="X6" s="104"/>
+      <c r="Y6" s="104"/>
+      <c r="Z6" s="104"/>
+      <c r="AA6" s="104"/>
+      <c r="AB6" s="104"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="108" t="e">
+      <c r="B7" s="105" t="e">
         <f aca="false">B1</f>
         <v>#REF!</v>
       </c>
-      <c r="C7" s="109" t="e">
+      <c r="C7" s="106" t="e">
         <f aca="false">#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D7" s="109"/>
-      <c r="E7" s="109"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="109"/>
-      <c r="J7" s="109"/>
-      <c r="K7" s="109"/>
-      <c r="L7" s="109"/>
-      <c r="M7" s="109"/>
-      <c r="N7" s="109"/>
-      <c r="O7" s="110"/>
-      <c r="P7" s="110"/>
-      <c r="Q7" s="106"/>
-      <c r="R7" s="107"/>
-      <c r="S7" s="107"/>
-      <c r="T7" s="107"/>
-      <c r="U7" s="107"/>
-      <c r="V7" s="107"/>
-      <c r="W7" s="107"/>
-      <c r="X7" s="107"/>
-      <c r="Y7" s="107"/>
-      <c r="Z7" s="107"/>
-      <c r="AA7" s="107"/>
-      <c r="AB7" s="107"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="106"/>
+      <c r="F7" s="106"/>
+      <c r="G7" s="106"/>
+      <c r="H7" s="106"/>
+      <c r="I7" s="106"/>
+      <c r="J7" s="106"/>
+      <c r="K7" s="106"/>
+      <c r="L7" s="106"/>
+      <c r="M7" s="106"/>
+      <c r="N7" s="106"/>
+      <c r="O7" s="107"/>
+      <c r="P7" s="107"/>
+      <c r="Q7" s="103"/>
+      <c r="R7" s="104"/>
+      <c r="S7" s="104"/>
+      <c r="T7" s="104"/>
+      <c r="U7" s="104"/>
+      <c r="V7" s="104"/>
+      <c r="W7" s="104"/>
+      <c r="X7" s="104"/>
+      <c r="Y7" s="104"/>
+      <c r="Z7" s="104"/>
+      <c r="AA7" s="104"/>
+      <c r="AB7" s="104"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -3817,113 +3858,113 @@
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="108" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="111"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="108"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="111"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
-      <c r="G6" s="111"/>
+      <c r="B6" s="108"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="108"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="112" t="s">
+      <c r="B8" s="109" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="112"/>
-      <c r="D8" s="112"/>
+      <c r="C8" s="109"/>
+      <c r="D8" s="109"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="113" t="s">
+      <c r="B9" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="114" t="n">
+      <c r="C9" s="111" t="n">
         <v>0.99</v>
       </c>
-      <c r="D9" s="114" t="n">
+      <c r="D9" s="111" t="n">
         <v>0.95</v>
       </c>
-      <c r="E9" s="114" t="n">
+      <c r="E9" s="111" t="n">
         <v>0.9</v>
       </c>
-      <c r="F9" s="114" t="n">
+      <c r="F9" s="111" t="n">
         <v>0.85</v>
       </c>
-      <c r="G9" s="113" t="s">
+      <c r="G9" s="110" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="115" t="n">
+      <c r="B10" s="112" t="n">
         <f aca="false">104%-0.000000000001</f>
         <v>1.039999999999</v>
       </c>
-      <c r="C10" s="114" t="n">
+      <c r="C10" s="111" t="n">
         <v>1.04</v>
       </c>
-      <c r="D10" s="114" t="n">
+      <c r="D10" s="111" t="n">
         <v>0.99</v>
       </c>
-      <c r="E10" s="114" t="n">
+      <c r="E10" s="111" t="n">
         <v>0.95</v>
       </c>
-      <c r="F10" s="114" t="n">
+      <c r="F10" s="111" t="n">
         <v>0.9</v>
       </c>
-      <c r="G10" s="114" t="n">
+      <c r="G10" s="111" t="n">
         <v>0.85</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="112" t="s">
+      <c r="B12" s="109" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="112"/>
-      <c r="D12" s="112"/>
+      <c r="C12" s="109"/>
+      <c r="D12" s="109"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="113"/>
-      <c r="C13" s="114" t="n">
+      <c r="B13" s="110"/>
+      <c r="C13" s="111" t="n">
         <v>0.96</v>
       </c>
-      <c r="D13" s="114" t="n">
+      <c r="D13" s="111" t="n">
         <v>1.01</v>
       </c>
-      <c r="E13" s="114" t="n">
+      <c r="E13" s="111" t="n">
         <v>1.05</v>
       </c>
-      <c r="F13" s="114" t="n">
+      <c r="F13" s="111" t="n">
         <v>1.1</v>
       </c>
-      <c r="G13" s="113" t="s">
+      <c r="G13" s="110" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="114" t="n">
+      <c r="B14" s="111" t="n">
         <v>0.96</v>
       </c>
-      <c r="C14" s="114" t="n">
+      <c r="C14" s="111" t="n">
         <v>1.01</v>
       </c>
-      <c r="D14" s="114" t="n">
+      <c r="D14" s="111" t="n">
         <v>1.05</v>
       </c>
-      <c r="E14" s="114" t="n">
+      <c r="E14" s="111" t="n">
         <v>1.1</v>
       </c>
-      <c r="F14" s="114" t="n">
+      <c r="F14" s="111" t="n">
         <v>1.15</v>
       </c>
-      <c r="G14" s="114" t="n">
+      <c r="G14" s="111" t="n">
         <v>1.15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajusta align de campo que comporta numero de documento
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/TEMPLATE_METAS.xlsx
+++ b/src/main/resources/templates/TEMPLATE_METAS.xlsx
@@ -998,45 +998,6 @@
   </cellStyleXfs>
   <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1290,42 +1251,6 @@
     <xf numFmtId="9" fontId="0" fillId="15" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="7" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="9" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="9" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="9" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="24" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1339,6 +1264,81 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="7" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="9" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="9" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="9" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1352,7 +1352,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2094,871 +2094,923 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="37.85546875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="14" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="4.85546875" style="14" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="14" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="14" customWidth="1"/>
-    <col min="12" max="12" width="15" style="14" customWidth="1"/>
-    <col min="13" max="13" width="18" style="14" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="14" customWidth="1"/>
-    <col min="15" max="15" width="32.85546875" style="15" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" style="14" customWidth="1"/>
-    <col min="17" max="1025" width="9.140625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="32.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" style="1" customWidth="1"/>
+    <col min="17" max="1025" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
+    <row r="1" spans="2:17" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
       <c r="L1" s="118"/>
       <c r="M1" s="118"/>
-      <c r="O1" s="15"/>
-    </row>
-    <row r="2" spans="2:17" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="2:17" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
       <c r="L2" s="118"/>
       <c r="M2" s="118"/>
-      <c r="O2" s="15"/>
+      <c r="O2" s="2"/>
     </row>
     <row r="3" spans="2:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="106"/>
+      <c r="J3" s="106"/>
+      <c r="K3" s="106"/>
+      <c r="L3" s="106"/>
+      <c r="M3" s="106"/>
     </row>
     <row r="4" spans="2:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23" t="s">
+      <c r="E4" s="9"/>
+      <c r="F4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="24" t="s">
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
+      <c r="K4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
+      <c r="L4" s="113"/>
+      <c r="M4" s="113"/>
     </row>
     <row r="5" spans="2:17" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
     </row>
     <row r="6" spans="2:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="106" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
+      <c r="C6" s="106"/>
+      <c r="D6" s="106"/>
+      <c r="E6" s="106"/>
+      <c r="F6" s="106"/>
+      <c r="G6" s="106"/>
+      <c r="H6" s="106"/>
+      <c r="I6" s="106"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="106"/>
+      <c r="L6" s="106"/>
+      <c r="M6" s="106"/>
     </row>
     <row r="7" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="107" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="108"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="109"/>
+      <c r="K7" s="109"/>
+      <c r="L7" s="109"/>
+      <c r="M7" s="109"/>
     </row>
     <row r="8" spans="2:17" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="30"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="36"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
     </row>
     <row r="9" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="36"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="110"/>
+      <c r="J9" s="110"/>
+      <c r="K9" s="110"/>
+      <c r="L9" s="110"/>
+      <c r="M9" s="110"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
     </row>
     <row r="10" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="36"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="36"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="103"/>
+      <c r="G10" s="103"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="104"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="104"/>
+      <c r="L10" s="104"/>
+      <c r="M10" s="104"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
     </row>
     <row r="11" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="36"/>
-      <c r="Q11" s="36"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="104"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="104"/>
+      <c r="L11" s="104"/>
+      <c r="M11" s="104"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
     </row>
     <row r="12" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="37"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="36"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="105"/>
+      <c r="G12" s="105"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="104"/>
+      <c r="J12" s="104"/>
+      <c r="K12" s="104"/>
+      <c r="L12" s="104"/>
+      <c r="M12" s="104"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
     </row>
     <row r="13" spans="2:17" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N13" s="36"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="36"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
     </row>
     <row r="14" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="36"/>
-      <c r="Q14" s="36"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="101"/>
+      <c r="F14" s="101"/>
+      <c r="G14" s="101"/>
+      <c r="H14" s="101"/>
+      <c r="I14" s="101"/>
+      <c r="J14" s="101"/>
+      <c r="K14" s="101"/>
+      <c r="L14" s="101"/>
+      <c r="M14" s="101"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
     </row>
     <row r="15" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="98" t="s">
+      <c r="D15" s="102"/>
+      <c r="E15" s="102"/>
+      <c r="F15" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="98"/>
-      <c r="H15" s="98" t="s">
+      <c r="G15" s="97"/>
+      <c r="H15" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="98"/>
-      <c r="J15" s="42" t="s">
+      <c r="I15" s="97"/>
+      <c r="J15" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="98" t="s">
+      <c r="K15" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="L15" s="98"/>
-      <c r="M15" s="42" t="s">
+      <c r="L15" s="97"/>
+      <c r="M15" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="36"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="36"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
     </row>
     <row r="16" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="43"/>
-      <c r="C16" s="99"/>
-      <c r="D16" s="99"/>
-      <c r="E16" s="99"/>
-      <c r="F16" s="99"/>
-      <c r="G16" s="99"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="100">
+      <c r="B16" s="30"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="89"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="90">
         <f>SUM(H16:H27)</f>
         <v>0</v>
       </c>
-      <c r="J16" s="45"/>
-      <c r="K16" s="101"/>
-      <c r="L16" s="101"/>
-      <c r="M16" s="47"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="36"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="99"/>
+      <c r="L16" s="99"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
     </row>
     <row r="17" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="48"/>
-      <c r="C17" s="99"/>
-      <c r="D17" s="99"/>
-      <c r="E17" s="99"/>
-      <c r="F17" s="99"/>
-      <c r="G17" s="99"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="100"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="101"/>
-      <c r="L17" s="101"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="36"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="36"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="99"/>
+      <c r="L17" s="99"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
     </row>
     <row r="18" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="48"/>
-      <c r="C18" s="99"/>
-      <c r="D18" s="99"/>
-      <c r="E18" s="99"/>
-      <c r="F18" s="99"/>
-      <c r="G18" s="99"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="100"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="101"/>
-      <c r="L18" s="101"/>
-      <c r="M18" s="47"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="36"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="89"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="90"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="99"/>
+      <c r="L18" s="99"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
     </row>
     <row r="19" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="48"/>
-      <c r="C19" s="99"/>
-      <c r="D19" s="99"/>
-      <c r="E19" s="99"/>
-      <c r="F19" s="99"/>
-      <c r="G19" s="99"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="100"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="101"/>
-      <c r="L19" s="101"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="36"/>
-      <c r="Q19" s="36"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
+      <c r="E19" s="89"/>
+      <c r="F19" s="89"/>
+      <c r="G19" s="89"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="90"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="99"/>
+      <c r="L19" s="99"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
     </row>
     <row r="20" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="48"/>
-      <c r="C20" s="99"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="99"/>
-      <c r="F20" s="99"/>
-      <c r="G20" s="99"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="100"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="90"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
     </row>
     <row r="21" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="48"/>
-      <c r="C21" s="99"/>
-      <c r="D21" s="99"/>
-      <c r="E21" s="99"/>
-      <c r="F21" s="99"/>
-      <c r="G21" s="99"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="100"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="46"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="36"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="89"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="89"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="90"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
     </row>
     <row r="22" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="48"/>
-      <c r="C22" s="102"/>
-      <c r="D22" s="102"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="102"/>
-      <c r="G22" s="102"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="100"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="101"/>
-      <c r="L22" s="101"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="36"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="92"/>
+      <c r="D22" s="92"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="92"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="90"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="99"/>
+      <c r="L22" s="99"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
     </row>
     <row r="23" spans="2:17" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="48" t="str">
+      <c r="B23" s="35" t="str">
         <f>IF(C23&lt;&gt;"",B22+1,"")</f>
         <v/>
       </c>
-      <c r="C23" s="102"/>
-      <c r="D23" s="102"/>
-      <c r="E23" s="102"/>
-      <c r="F23" s="102"/>
-      <c r="G23" s="102"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="100"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="103"/>
-      <c r="L23" s="103"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="36"/>
-      <c r="Q23" s="36"/>
+      <c r="C23" s="92"/>
+      <c r="D23" s="92"/>
+      <c r="E23" s="92"/>
+      <c r="F23" s="92"/>
+      <c r="G23" s="92"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="90"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="100"/>
+      <c r="L23" s="100"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
     </row>
     <row r="24" spans="2:17" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="48" t="str">
+      <c r="B24" s="35" t="str">
         <f>IF(C24&lt;&gt;"",B23+1,"")</f>
         <v/>
       </c>
-      <c r="C24" s="102"/>
-      <c r="D24" s="102"/>
-      <c r="E24" s="102"/>
-      <c r="F24" s="102"/>
-      <c r="G24" s="102"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="100"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="104"/>
-      <c r="L24" s="104"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="37"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="36"/>
+      <c r="C24" s="92"/>
+      <c r="D24" s="92"/>
+      <c r="E24" s="92"/>
+      <c r="F24" s="92"/>
+      <c r="G24" s="92"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="90"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="98"/>
+      <c r="L24" s="98"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
     </row>
     <row r="25" spans="2:17" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="48" t="str">
+      <c r="B25" s="35" t="str">
         <f>IF(C25&lt;&gt;"",B24+1,"")</f>
         <v/>
       </c>
-      <c r="C25" s="102"/>
-      <c r="D25" s="102"/>
-      <c r="E25" s="102"/>
-      <c r="F25" s="102"/>
-      <c r="G25" s="102"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="100"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="104"/>
-      <c r="L25" s="104"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="36"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="36"/>
-      <c r="Q25" s="36"/>
+      <c r="C25" s="92"/>
+      <c r="D25" s="92"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="92"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="90"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="98"/>
+      <c r="L25" s="98"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
     </row>
     <row r="26" spans="2:17" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="48" t="str">
+      <c r="B26" s="35" t="str">
         <f>IF(C26&lt;&gt;"",B25+1,"")</f>
         <v/>
       </c>
-      <c r="C26" s="102"/>
-      <c r="D26" s="102"/>
-      <c r="E26" s="102"/>
-      <c r="F26" s="102"/>
-      <c r="G26" s="102"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="100"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="104"/>
-      <c r="L26" s="104"/>
-      <c r="M26" s="47"/>
-      <c r="N26" s="36"/>
-      <c r="O26" s="37"/>
-      <c r="P26" s="36"/>
-      <c r="Q26" s="36"/>
+      <c r="C26" s="92"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="92"/>
+      <c r="F26" s="92"/>
+      <c r="G26" s="92"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="90"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="98"/>
+      <c r="L26" s="98"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="23"/>
     </row>
     <row r="27" spans="2:17" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="52" t="str">
+      <c r="B27" s="39" t="str">
         <f>IF(C27&lt;&gt;"",B26+1,"")</f>
         <v/>
       </c>
-      <c r="C27" s="105"/>
-      <c r="D27" s="105"/>
-      <c r="E27" s="105"/>
-      <c r="F27" s="105"/>
-      <c r="G27" s="105"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="100"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="106"/>
-      <c r="L27" s="106"/>
-      <c r="M27" s="55"/>
-      <c r="N27" s="36"/>
-      <c r="O27" s="37"/>
-      <c r="P27" s="36"/>
-      <c r="Q27" s="36"/>
+      <c r="C27" s="93"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="93"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="93"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="90"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="94"/>
+      <c r="L27" s="94"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
     </row>
     <row r="28" spans="2:17" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N28" s="36"/>
-      <c r="O28" s="37"/>
-      <c r="P28" s="36"/>
-      <c r="Q28" s="36"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
     </row>
     <row r="29" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="107" t="s">
+      <c r="B29" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="107"/>
-      <c r="D29" s="107"/>
-      <c r="E29" s="107"/>
-      <c r="F29" s="107"/>
-      <c r="G29" s="107"/>
-      <c r="H29" s="107"/>
-      <c r="I29" s="107"/>
-      <c r="J29" s="107"/>
-      <c r="K29" s="107"/>
-      <c r="L29" s="107"/>
-      <c r="M29" s="107"/>
-      <c r="N29" s="36"/>
-      <c r="O29" s="37"/>
-      <c r="P29" s="36"/>
-      <c r="Q29" s="36"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="95"/>
+      <c r="F29" s="95"/>
+      <c r="G29" s="95"/>
+      <c r="H29" s="95"/>
+      <c r="I29" s="95"/>
+      <c r="J29" s="95"/>
+      <c r="K29" s="95"/>
+      <c r="L29" s="95"/>
+      <c r="M29" s="95"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
     </row>
     <row r="30" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="108" t="s">
+      <c r="C30" s="28"/>
+      <c r="D30" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="E30" s="108"/>
-      <c r="F30" s="98" t="s">
+      <c r="E30" s="96"/>
+      <c r="F30" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="G30" s="98"/>
-      <c r="H30" s="98" t="s">
+      <c r="G30" s="97"/>
+      <c r="H30" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="I30" s="98"/>
-      <c r="J30" s="42" t="s">
+      <c r="I30" s="97"/>
+      <c r="J30" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="K30" s="98" t="s">
+      <c r="K30" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="L30" s="98"/>
-      <c r="M30" s="42" t="s">
+      <c r="L30" s="97"/>
+      <c r="M30" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="N30" s="36"/>
-      <c r="O30" s="37"/>
-      <c r="P30" s="36"/>
-      <c r="Q30" s="36"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="23"/>
     </row>
     <row r="31" spans="2:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="43"/>
-      <c r="C31" s="99"/>
-      <c r="D31" s="99"/>
-      <c r="E31" s="99"/>
-      <c r="F31" s="99"/>
-      <c r="G31" s="99"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="100">
+      <c r="B31" s="30"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="89"/>
+      <c r="G31" s="89"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="90">
         <f>SUM(H31:H37)</f>
         <v>0</v>
       </c>
-      <c r="J31" s="45"/>
-      <c r="K31" s="109"/>
-      <c r="L31" s="109"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="36"/>
-      <c r="O31" s="37"/>
-      <c r="P31" s="36"/>
-      <c r="Q31" s="36"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="91"/>
+      <c r="L31" s="91"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="23"/>
+      <c r="Q31" s="23"/>
     </row>
     <row r="32" spans="2:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="48"/>
-      <c r="C32" s="102"/>
-      <c r="D32" s="102"/>
-      <c r="E32" s="102"/>
-      <c r="F32" s="102"/>
-      <c r="G32" s="102"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="100"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="109"/>
-      <c r="L32" s="109"/>
-      <c r="M32" s="47"/>
-      <c r="N32" s="36"/>
-      <c r="O32" s="37"/>
-      <c r="P32" s="36"/>
-      <c r="Q32" s="36"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="92"/>
+      <c r="D32" s="92"/>
+      <c r="E32" s="92"/>
+      <c r="F32" s="92"/>
+      <c r="G32" s="92"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="90"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="91"/>
+      <c r="L32" s="91"/>
+      <c r="M32" s="34"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
     </row>
     <row r="33" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="48"/>
-      <c r="C33" s="102"/>
-      <c r="D33" s="102"/>
-      <c r="E33" s="102"/>
-      <c r="F33" s="102"/>
-      <c r="G33" s="102"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="100"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="109"/>
-      <c r="L33" s="109"/>
-      <c r="M33" s="47"/>
-      <c r="N33" s="36"/>
-      <c r="O33" s="37"/>
-      <c r="P33" s="36"/>
-      <c r="Q33" s="36"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="92"/>
+      <c r="D33" s="92"/>
+      <c r="E33" s="92"/>
+      <c r="F33" s="92"/>
+      <c r="G33" s="92"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="90"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="91"/>
+      <c r="L33" s="91"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23"/>
     </row>
     <row r="34" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="48"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="44"/>
-      <c r="I34" s="100"/>
-      <c r="J34" s="45"/>
-      <c r="K34" s="57"/>
-      <c r="L34" s="57"/>
-      <c r="M34" s="47"/>
-      <c r="N34" s="36"/>
-      <c r="O34" s="37"/>
-      <c r="P34" s="36"/>
-      <c r="Q34" s="36"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="90"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="44"/>
+      <c r="M34" s="34"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="24"/>
+      <c r="P34" s="23"/>
+      <c r="Q34" s="23"/>
     </row>
     <row r="35" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="48"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="100"/>
-      <c r="J35" s="45"/>
-      <c r="K35" s="57"/>
-      <c r="L35" s="57"/>
-      <c r="M35" s="47"/>
-      <c r="N35" s="36"/>
-      <c r="O35" s="37"/>
-      <c r="P35" s="36"/>
-      <c r="Q35" s="36"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="90"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="44"/>
+      <c r="M35" s="34"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="24"/>
+      <c r="P35" s="23"/>
+      <c r="Q35" s="23"/>
     </row>
     <row r="36" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="48"/>
-      <c r="C36" s="102"/>
-      <c r="D36" s="102"/>
-      <c r="E36" s="102"/>
-      <c r="F36" s="102"/>
-      <c r="G36" s="102"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="100"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="109"/>
-      <c r="L36" s="109"/>
-      <c r="M36" s="47"/>
-      <c r="N36" s="36"/>
-      <c r="O36" s="37"/>
-      <c r="P36" s="36"/>
-      <c r="Q36" s="36"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="92"/>
+      <c r="D36" s="92"/>
+      <c r="E36" s="92"/>
+      <c r="F36" s="92"/>
+      <c r="G36" s="92"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="90"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="91"/>
+      <c r="L36" s="91"/>
+      <c r="M36" s="34"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="23"/>
+      <c r="Q36" s="23"/>
     </row>
     <row r="37" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="48"/>
-      <c r="C37" s="102"/>
-      <c r="D37" s="102"/>
-      <c r="E37" s="102"/>
-      <c r="F37" s="102"/>
-      <c r="G37" s="102"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="100"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="109"/>
-      <c r="L37" s="109"/>
-      <c r="M37" s="47"/>
-      <c r="N37" s="36"/>
-      <c r="O37" s="37"/>
-      <c r="P37" s="36"/>
-      <c r="Q37" s="36"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="92"/>
+      <c r="D37" s="92"/>
+      <c r="E37" s="92"/>
+      <c r="F37" s="92"/>
+      <c r="G37" s="92"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="90"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="91"/>
+      <c r="L37" s="91"/>
+      <c r="M37" s="34"/>
+      <c r="N37" s="23"/>
+      <c r="O37" s="24"/>
+      <c r="P37" s="23"/>
+      <c r="Q37" s="23"/>
     </row>
     <row r="38" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="36"/>
-      <c r="B38" s="58"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
-      <c r="F38" s="58"/>
-      <c r="G38" s="59" t="s">
+      <c r="A38" s="23"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="H38" s="60">
+      <c r="H38" s="47">
         <f>I31+I16</f>
         <v>0</v>
       </c>
-      <c r="I38" s="58"/>
-      <c r="J38" s="58"/>
-      <c r="K38" s="58"/>
-      <c r="L38" s="58"/>
-      <c r="M38" s="58"/>
-      <c r="N38" s="36"/>
-      <c r="O38" s="37"/>
-      <c r="P38" s="36"/>
-      <c r="Q38" s="36"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="45"/>
+      <c r="M38" s="45"/>
+      <c r="N38" s="23"/>
+      <c r="O38" s="24"/>
+      <c r="P38" s="23"/>
+      <c r="Q38" s="23"/>
     </row>
     <row r="39" spans="1:17" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="110"/>
-      <c r="G39" s="110"/>
-      <c r="H39" s="110"/>
-      <c r="I39" s="110"/>
-      <c r="J39" s="110"/>
-      <c r="K39" s="110"/>
-      <c r="L39" s="110"/>
-      <c r="M39" s="110"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="37"/>
-      <c r="P39" s="36"/>
-      <c r="Q39" s="36"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="85"/>
+      <c r="G39" s="85"/>
+      <c r="H39" s="85"/>
+      <c r="I39" s="85"/>
+      <c r="J39" s="85"/>
+      <c r="K39" s="85"/>
+      <c r="L39" s="85"/>
+      <c r="M39" s="85"/>
+      <c r="N39" s="23"/>
+      <c r="O39" s="24"/>
+      <c r="P39" s="23"/>
+      <c r="Q39" s="23"/>
     </row>
     <row r="40" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="111" t="s">
+      <c r="B40" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="111"/>
-      <c r="D40" s="111"/>
-      <c r="E40" s="111"/>
-      <c r="F40" s="111"/>
-      <c r="G40" s="111"/>
-      <c r="H40" s="111"/>
-      <c r="I40" s="111"/>
-      <c r="J40" s="111"/>
-      <c r="K40" s="111"/>
-      <c r="L40" s="111"/>
-      <c r="M40" s="111"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="86"/>
+      <c r="G40" s="86"/>
+      <c r="H40" s="86"/>
+      <c r="I40" s="86"/>
+      <c r="J40" s="86"/>
+      <c r="K40" s="86"/>
+      <c r="L40" s="86"/>
+      <c r="M40" s="86"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B41" s="61"/>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="61"/>
-      <c r="I41" s="61"/>
-      <c r="J41" s="61"/>
-      <c r="K41" s="61"/>
-      <c r="L41" s="61"/>
-      <c r="M41" s="61"/>
-    </row>
-    <row r="42" spans="1:17" s="62" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="63"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="64"/>
-      <c r="F42" s="112"/>
-      <c r="G42" s="112"/>
-      <c r="H42" s="112"/>
-      <c r="I42" s="112"/>
-      <c r="J42" s="66"/>
-      <c r="K42" s="66"/>
-      <c r="L42" s="66"/>
-      <c r="M42" s="66"/>
-      <c r="O42" s="67"/>
-    </row>
-    <row r="43" spans="1:17" s="62" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="63"/>
-      <c r="C43" s="63"/>
-      <c r="D43" s="63"/>
-      <c r="E43" s="63"/>
-      <c r="F43" s="113" t="s">
+      <c r="B41" s="48"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="48"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="48"/>
+      <c r="K41" s="48"/>
+      <c r="L41" s="48"/>
+      <c r="M41" s="48"/>
+    </row>
+    <row r="42" spans="1:17" s="49" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="50"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="87"/>
+      <c r="G42" s="87"/>
+      <c r="H42" s="87"/>
+      <c r="I42" s="87"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="53"/>
+      <c r="L42" s="53"/>
+      <c r="M42" s="53"/>
+      <c r="O42" s="54"/>
+    </row>
+    <row r="43" spans="1:17" s="49" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="50"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="G43" s="113"/>
-      <c r="H43" s="66"/>
-      <c r="I43" s="66"/>
-      <c r="J43" s="113" t="s">
+      <c r="G43" s="88"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="53"/>
+      <c r="J43" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="K43" s="113"/>
-      <c r="L43" s="113"/>
-      <c r="M43" s="113"/>
-      <c r="O43" s="67"/>
-    </row>
-    <row r="44" spans="1:17" s="62" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="63"/>
-      <c r="C44" s="63"/>
-      <c r="D44" s="63"/>
-      <c r="E44" s="68"/>
-      <c r="F44" s="63"/>
-      <c r="G44" s="63"/>
-      <c r="H44" s="63"/>
-      <c r="I44" s="63"/>
-      <c r="J44" s="65"/>
-      <c r="K44" s="65"/>
-      <c r="L44" s="65"/>
-      <c r="M44" s="65"/>
-      <c r="O44" s="67"/>
-    </row>
-    <row r="45" spans="1:17" s="62" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="69"/>
-      <c r="C45" s="69"/>
-      <c r="D45" s="70"/>
-      <c r="E45" s="71"/>
-      <c r="F45" s="72"/>
-      <c r="G45" s="72"/>
-      <c r="H45" s="72"/>
-      <c r="I45" s="72"/>
-      <c r="J45" s="72"/>
-      <c r="K45" s="72"/>
-      <c r="L45" s="72"/>
-      <c r="M45" s="72"/>
-      <c r="O45" s="67"/>
-    </row>
-    <row r="46" spans="1:17" s="62" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="73" t="str">
+      <c r="K43" s="88"/>
+      <c r="L43" s="88"/>
+      <c r="M43" s="88"/>
+      <c r="O43" s="54"/>
+    </row>
+    <row r="44" spans="1:17" s="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="52"/>
+      <c r="K44" s="52"/>
+      <c r="L44" s="52"/>
+      <c r="M44" s="52"/>
+      <c r="O44" s="54"/>
+    </row>
+    <row r="45" spans="1:17" s="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="56"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="58"/>
+      <c r="F45" s="59"/>
+      <c r="G45" s="59"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
+      <c r="K45" s="59"/>
+      <c r="L45" s="59"/>
+      <c r="M45" s="59"/>
+      <c r="O45" s="54"/>
+    </row>
+    <row r="46" spans="1:17" s="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="60" t="str">
         <f ca="1">CELL("FILENAME")</f>
         <v>C:\Users\idealit\Documents\projetos\plr\src\main\resources\templates\[TEMPLATE_METAS.xlsx]FOLHA METAS</v>
       </c>
-      <c r="C46" s="74"/>
-      <c r="E46" s="75"/>
-      <c r="O46" s="67"/>
+      <c r="C46" s="61"/>
+      <c r="E46" s="62"/>
+      <c r="O46" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="F39:M39"/>
-    <mergeCell ref="B40:M40"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="D1:K2"/>
+    <mergeCell ref="L1:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I7:M7"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="I16:I27"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="B29:M29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="K30:L30"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="I31:I37"/>
@@ -2975,63 +3027,11 @@
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="F37:G37"/>
     <mergeCell ref="K37:L37"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="B29:M29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="I16:I27"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="I12:M12"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="I7:M7"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="D1:K2"/>
-    <mergeCell ref="L1:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="F39:M39"/>
+    <mergeCell ref="B40:M40"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="J43:M43"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.118055555555556" right="0.118055555555556" top="0.196527777777778" bottom="0.196527777777778" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3053,17 +3053,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="76" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="76" customWidth="1"/>
-    <col min="3" max="14" width="13.7109375" style="76" customWidth="1"/>
-    <col min="15" max="15" width="1.140625" style="76" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" style="76" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" style="76" customWidth="1"/>
-    <col min="18" max="1025" width="9.140625" style="76" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" style="63" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="63" customWidth="1"/>
+    <col min="3" max="14" width="13.7109375" style="63" customWidth="1"/>
+    <col min="15" max="15" width="1.140625" style="63" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" style="63" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" style="63" customWidth="1"/>
+    <col min="18" max="1025" width="9.140625" style="63" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="77" t="e">
+      <c r="B1" s="64" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
@@ -3087,150 +3087,150 @@
       <c r="Q1" s="114"/>
     </row>
     <row r="2" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="78" t="s">
+      <c r="E2" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="78" t="s">
+      <c r="G2" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="78" t="s">
+      <c r="H2" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="78" t="s">
+      <c r="I2" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="78" t="s">
+      <c r="J2" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="78" t="s">
+      <c r="K2" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="78" t="s">
+      <c r="L2" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="78" t="s">
+      <c r="M2" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="78" t="s">
+      <c r="N2" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="79"/>
-      <c r="P2" s="78" t="s">
+      <c r="O2" s="66"/>
+      <c r="P2" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="78" t="s">
+      <c r="Q2" s="65" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="83">
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="70">
         <f>SUM(C3:N3)</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="84">
+      <c r="Q3" s="71">
         <f>IFERROR(AVERAGE(C3:N3),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="87">
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="74">
         <f>SUM(C4:N4)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="88">
+      <c r="Q4" s="75">
         <f>IFERROR(AVERAGE(C4:N4),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H5" s="89"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="90"/>
-      <c r="N5" s="90"/>
-      <c r="O5" s="91"/>
-      <c r="P5" s="91"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="92"/>
-      <c r="S5" s="92"/>
-      <c r="T5" s="92"/>
-      <c r="U5" s="92"/>
-      <c r="V5" s="92"/>
-      <c r="W5" s="92"/>
-      <c r="X5" s="92"/>
-      <c r="Y5" s="92"/>
-      <c r="Z5" s="92"/>
-      <c r="AA5" s="92"/>
-      <c r="AB5" s="92"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="79"/>
+      <c r="T5" s="79"/>
+      <c r="U5" s="79"/>
+      <c r="V5" s="79"/>
+      <c r="W5" s="79"/>
+      <c r="X5" s="79"/>
+      <c r="Y5" s="79"/>
+      <c r="Z5" s="79"/>
+      <c r="AA5" s="79"/>
+      <c r="AB5" s="79"/>
     </row>
     <row r="6" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H6" s="89"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-      <c r="O6" s="91"/>
-      <c r="P6" s="91"/>
-      <c r="Q6" s="91"/>
-      <c r="R6" s="92"/>
-      <c r="S6" s="92"/>
-      <c r="T6" s="92"/>
-      <c r="U6" s="92"/>
-      <c r="V6" s="92"/>
-      <c r="W6" s="92"/>
-      <c r="X6" s="92"/>
-      <c r="Y6" s="92"/>
-      <c r="Z6" s="92"/>
-      <c r="AA6" s="92"/>
-      <c r="AB6" s="92"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="79"/>
+      <c r="S6" s="79"/>
+      <c r="T6" s="79"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="79"/>
+      <c r="X6" s="79"/>
+      <c r="Y6" s="79"/>
+      <c r="Z6" s="79"/>
+      <c r="AA6" s="79"/>
+      <c r="AB6" s="79"/>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B7" s="93" t="e">
+      <c r="B7" s="80" t="e">
         <f>B1</f>
         <v>#REF!</v>
       </c>
@@ -3249,20 +3249,20 @@
       <c r="L7" s="115"/>
       <c r="M7" s="115"/>
       <c r="N7" s="115"/>
-      <c r="O7" s="94"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="91"/>
-      <c r="R7" s="92"/>
-      <c r="S7" s="92"/>
-      <c r="T7" s="92"/>
-      <c r="U7" s="92"/>
-      <c r="V7" s="92"/>
-      <c r="W7" s="92"/>
-      <c r="X7" s="92"/>
-      <c r="Y7" s="92"/>
-      <c r="Z7" s="92"/>
-      <c r="AA7" s="92"/>
-      <c r="AB7" s="92"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="81"/>
+      <c r="Q7" s="78"/>
+      <c r="R7" s="79"/>
+      <c r="S7" s="79"/>
+      <c r="T7" s="79"/>
+      <c r="U7" s="79"/>
+      <c r="V7" s="79"/>
+      <c r="W7" s="79"/>
+      <c r="X7" s="79"/>
+      <c r="Y7" s="79"/>
+      <c r="Z7" s="79"/>
+      <c r="AA7" s="79"/>
+      <c r="AB7" s="79"/>
     </row>
     <row r="8" spans="2:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -3285,17 +3285,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="76" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="76" customWidth="1"/>
-    <col min="3" max="14" width="13.7109375" style="76" customWidth="1"/>
-    <col min="15" max="15" width="1.140625" style="76" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" style="76" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" style="76" customWidth="1"/>
-    <col min="18" max="1025" width="9.140625" style="76" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" style="63" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="63" customWidth="1"/>
+    <col min="3" max="14" width="13.7109375" style="63" customWidth="1"/>
+    <col min="15" max="15" width="1.140625" style="63" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" style="63" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" style="63" customWidth="1"/>
+    <col min="18" max="1025" width="9.140625" style="63" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="77" t="e">
+      <c r="B1" s="64" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
@@ -3319,150 +3319,150 @@
       <c r="Q1" s="114"/>
     </row>
     <row r="2" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="78" t="s">
+      <c r="E2" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="78" t="s">
+      <c r="G2" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="78" t="s">
+      <c r="H2" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="78" t="s">
+      <c r="I2" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="78" t="s">
+      <c r="J2" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="78" t="s">
+      <c r="K2" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="78" t="s">
+      <c r="L2" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="78" t="s">
+      <c r="M2" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="78" t="s">
+      <c r="N2" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="79"/>
-      <c r="P2" s="78" t="s">
+      <c r="O2" s="66"/>
+      <c r="P2" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="78" t="s">
+      <c r="Q2" s="65" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="83">
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="70">
         <f>SUM(C3:N3)</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="84">
+      <c r="Q3" s="71">
         <f>IFERROR(AVERAGE(C3:N3),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="87">
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="74">
         <f>SUM(C4:N4)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="88">
+      <c r="Q4" s="75">
         <f>IFERROR(AVERAGE(C4:N4),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H5" s="89"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="90"/>
-      <c r="N5" s="90"/>
-      <c r="O5" s="91"/>
-      <c r="P5" s="91"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="92"/>
-      <c r="S5" s="92"/>
-      <c r="T5" s="92"/>
-      <c r="U5" s="92"/>
-      <c r="V5" s="92"/>
-      <c r="W5" s="92"/>
-      <c r="X5" s="92"/>
-      <c r="Y5" s="92"/>
-      <c r="Z5" s="92"/>
-      <c r="AA5" s="92"/>
-      <c r="AB5" s="92"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="79"/>
+      <c r="T5" s="79"/>
+      <c r="U5" s="79"/>
+      <c r="V5" s="79"/>
+      <c r="W5" s="79"/>
+      <c r="X5" s="79"/>
+      <c r="Y5" s="79"/>
+      <c r="Z5" s="79"/>
+      <c r="AA5" s="79"/>
+      <c r="AB5" s="79"/>
     </row>
     <row r="6" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H6" s="89"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-      <c r="O6" s="91"/>
-      <c r="P6" s="91"/>
-      <c r="Q6" s="91"/>
-      <c r="R6" s="92"/>
-      <c r="S6" s="92"/>
-      <c r="T6" s="92"/>
-      <c r="U6" s="92"/>
-      <c r="V6" s="92"/>
-      <c r="W6" s="92"/>
-      <c r="X6" s="92"/>
-      <c r="Y6" s="92"/>
-      <c r="Z6" s="92"/>
-      <c r="AA6" s="92"/>
-      <c r="AB6" s="92"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="79"/>
+      <c r="S6" s="79"/>
+      <c r="T6" s="79"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="79"/>
+      <c r="X6" s="79"/>
+      <c r="Y6" s="79"/>
+      <c r="Z6" s="79"/>
+      <c r="AA6" s="79"/>
+      <c r="AB6" s="79"/>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B7" s="93" t="e">
+      <c r="B7" s="80" t="e">
         <f>B1</f>
         <v>#REF!</v>
       </c>
@@ -3481,20 +3481,20 @@
       <c r="L7" s="115"/>
       <c r="M7" s="115"/>
       <c r="N7" s="115"/>
-      <c r="O7" s="94"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="91"/>
-      <c r="R7" s="92"/>
-      <c r="S7" s="92"/>
-      <c r="T7" s="92"/>
-      <c r="U7" s="92"/>
-      <c r="V7" s="92"/>
-      <c r="W7" s="92"/>
-      <c r="X7" s="92"/>
-      <c r="Y7" s="92"/>
-      <c r="Z7" s="92"/>
-      <c r="AA7" s="92"/>
-      <c r="AB7" s="92"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="81"/>
+      <c r="Q7" s="78"/>
+      <c r="R7" s="79"/>
+      <c r="S7" s="79"/>
+      <c r="T7" s="79"/>
+      <c r="U7" s="79"/>
+      <c r="V7" s="79"/>
+      <c r="W7" s="79"/>
+      <c r="X7" s="79"/>
+      <c r="Y7" s="79"/>
+      <c r="Z7" s="79"/>
+      <c r="AA7" s="79"/>
+      <c r="AB7" s="79"/>
     </row>
     <row r="8" spans="2:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -3517,17 +3517,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="76" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="76" customWidth="1"/>
-    <col min="3" max="14" width="13.7109375" style="76" customWidth="1"/>
-    <col min="15" max="15" width="1.140625" style="76" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" style="76" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" style="76" customWidth="1"/>
-    <col min="18" max="1025" width="9.140625" style="76" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" style="63" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="63" customWidth="1"/>
+    <col min="3" max="14" width="13.7109375" style="63" customWidth="1"/>
+    <col min="15" max="15" width="1.140625" style="63" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" style="63" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" style="63" customWidth="1"/>
+    <col min="18" max="1025" width="9.140625" style="63" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="77" t="e">
+      <c r="B1" s="64" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
@@ -3551,154 +3551,154 @@
       <c r="Q1" s="114"/>
     </row>
     <row r="2" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="76" t="e">
+      <c r="B2" s="63" t="e">
         <f>'FOLHA METAS'!C26:G26</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="78" t="s">
+      <c r="E2" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="78" t="s">
+      <c r="G2" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="78" t="s">
+      <c r="H2" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="78" t="s">
+      <c r="I2" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="78" t="s">
+      <c r="J2" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="78" t="s">
+      <c r="K2" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="78" t="s">
+      <c r="L2" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="78" t="s">
+      <c r="M2" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="78" t="s">
+      <c r="N2" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="79"/>
-      <c r="P2" s="78" t="s">
+      <c r="O2" s="66"/>
+      <c r="P2" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="78" t="s">
+      <c r="Q2" s="65" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="83">
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="70">
         <f>SUM(C3:N3)</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="84">
+      <c r="Q3" s="71">
         <f>IFERROR(AVERAGE(C3:N3),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="87">
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="74">
         <f>SUM(C4:N4)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="88">
+      <c r="Q4" s="75">
         <f>IFERROR(AVERAGE(C4:N4),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H5" s="89"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="90"/>
-      <c r="N5" s="90"/>
-      <c r="O5" s="91"/>
-      <c r="P5" s="91"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="92"/>
-      <c r="S5" s="92"/>
-      <c r="T5" s="92"/>
-      <c r="U5" s="92"/>
-      <c r="V5" s="92"/>
-      <c r="W5" s="92"/>
-      <c r="X5" s="92"/>
-      <c r="Y5" s="92"/>
-      <c r="Z5" s="92"/>
-      <c r="AA5" s="92"/>
-      <c r="AB5" s="92"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="79"/>
+      <c r="T5" s="79"/>
+      <c r="U5" s="79"/>
+      <c r="V5" s="79"/>
+      <c r="W5" s="79"/>
+      <c r="X5" s="79"/>
+      <c r="Y5" s="79"/>
+      <c r="Z5" s="79"/>
+      <c r="AA5" s="79"/>
+      <c r="AB5" s="79"/>
     </row>
     <row r="6" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H6" s="89"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-      <c r="O6" s="91"/>
-      <c r="P6" s="91"/>
-      <c r="Q6" s="91"/>
-      <c r="R6" s="92"/>
-      <c r="S6" s="92"/>
-      <c r="T6" s="92"/>
-      <c r="U6" s="92"/>
-      <c r="V6" s="92"/>
-      <c r="W6" s="92"/>
-      <c r="X6" s="92"/>
-      <c r="Y6" s="92"/>
-      <c r="Z6" s="92"/>
-      <c r="AA6" s="92"/>
-      <c r="AB6" s="92"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="79"/>
+      <c r="S6" s="79"/>
+      <c r="T6" s="79"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="79"/>
+      <c r="X6" s="79"/>
+      <c r="Y6" s="79"/>
+      <c r="Z6" s="79"/>
+      <c r="AA6" s="79"/>
+      <c r="AB6" s="79"/>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B7" s="93" t="e">
+      <c r="B7" s="80" t="e">
         <f>B1</f>
         <v>#REF!</v>
       </c>
@@ -3717,20 +3717,20 @@
       <c r="L7" s="115"/>
       <c r="M7" s="115"/>
       <c r="N7" s="115"/>
-      <c r="O7" s="94"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="91"/>
-      <c r="R7" s="92"/>
-      <c r="S7" s="92"/>
-      <c r="T7" s="92"/>
-      <c r="U7" s="92"/>
-      <c r="V7" s="92"/>
-      <c r="W7" s="92"/>
-      <c r="X7" s="92"/>
-      <c r="Y7" s="92"/>
-      <c r="Z7" s="92"/>
-      <c r="AA7" s="92"/>
-      <c r="AB7" s="92"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="81"/>
+      <c r="Q7" s="78"/>
+      <c r="R7" s="79"/>
+      <c r="S7" s="79"/>
+      <c r="T7" s="79"/>
+      <c r="U7" s="79"/>
+      <c r="V7" s="79"/>
+      <c r="W7" s="79"/>
+      <c r="X7" s="79"/>
+      <c r="Y7" s="79"/>
+      <c r="Z7" s="79"/>
+      <c r="AA7" s="79"/>
+      <c r="AB7" s="79"/>
     </row>
     <row r="8" spans="2:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -3753,17 +3753,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="76" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="76" customWidth="1"/>
-    <col min="3" max="14" width="13.7109375" style="76" customWidth="1"/>
-    <col min="15" max="15" width="1.140625" style="76" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" style="76" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" style="76" customWidth="1"/>
-    <col min="18" max="1025" width="9.140625" style="76" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" style="63" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="63" customWidth="1"/>
+    <col min="3" max="14" width="13.7109375" style="63" customWidth="1"/>
+    <col min="15" max="15" width="1.140625" style="63" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" style="63" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" style="63" customWidth="1"/>
+    <col min="18" max="1025" width="9.140625" style="63" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="77" t="e">
+      <c r="B1" s="64" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
@@ -3787,150 +3787,150 @@
       <c r="Q1" s="114"/>
     </row>
     <row r="2" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="78" t="s">
+      <c r="E2" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="78" t="s">
+      <c r="G2" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="78" t="s">
+      <c r="H2" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="78" t="s">
+      <c r="I2" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="78" t="s">
+      <c r="J2" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="78" t="s">
+      <c r="K2" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="78" t="s">
+      <c r="L2" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="78" t="s">
+      <c r="M2" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="78" t="s">
+      <c r="N2" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="79"/>
-      <c r="P2" s="78" t="s">
+      <c r="O2" s="66"/>
+      <c r="P2" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="78" t="s">
+      <c r="Q2" s="65" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="83">
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="70">
         <f>SUM(C3:N3)</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="84">
+      <c r="Q3" s="71">
         <f>IFERROR(AVERAGE(C3:N3),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="87">
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="74">
         <f>SUM(C4:N4)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="88">
+      <c r="Q4" s="75">
         <f>IFERROR(AVERAGE(C4:N4),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H5" s="89"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="90"/>
-      <c r="N5" s="90"/>
-      <c r="O5" s="91"/>
-      <c r="P5" s="91"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="92"/>
-      <c r="S5" s="92"/>
-      <c r="T5" s="92"/>
-      <c r="U5" s="92"/>
-      <c r="V5" s="92"/>
-      <c r="W5" s="92"/>
-      <c r="X5" s="92"/>
-      <c r="Y5" s="92"/>
-      <c r="Z5" s="92"/>
-      <c r="AA5" s="92"/>
-      <c r="AB5" s="92"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="79"/>
+      <c r="T5" s="79"/>
+      <c r="U5" s="79"/>
+      <c r="V5" s="79"/>
+      <c r="W5" s="79"/>
+      <c r="X5" s="79"/>
+      <c r="Y5" s="79"/>
+      <c r="Z5" s="79"/>
+      <c r="AA5" s="79"/>
+      <c r="AB5" s="79"/>
     </row>
     <row r="6" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H6" s="89"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-      <c r="O6" s="91"/>
-      <c r="P6" s="91"/>
-      <c r="Q6" s="91"/>
-      <c r="R6" s="92"/>
-      <c r="S6" s="92"/>
-      <c r="T6" s="92"/>
-      <c r="U6" s="92"/>
-      <c r="V6" s="92"/>
-      <c r="W6" s="92"/>
-      <c r="X6" s="92"/>
-      <c r="Y6" s="92"/>
-      <c r="Z6" s="92"/>
-      <c r="AA6" s="92"/>
-      <c r="AB6" s="92"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="79"/>
+      <c r="S6" s="79"/>
+      <c r="T6" s="79"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="79"/>
+      <c r="X6" s="79"/>
+      <c r="Y6" s="79"/>
+      <c r="Z6" s="79"/>
+      <c r="AA6" s="79"/>
+      <c r="AB6" s="79"/>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B7" s="93" t="e">
+      <c r="B7" s="80" t="e">
         <f>B1</f>
         <v>#REF!</v>
       </c>
@@ -3949,20 +3949,20 @@
       <c r="L7" s="115"/>
       <c r="M7" s="115"/>
       <c r="N7" s="115"/>
-      <c r="O7" s="94"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="91"/>
-      <c r="R7" s="92"/>
-      <c r="S7" s="92"/>
-      <c r="T7" s="92"/>
-      <c r="U7" s="92"/>
-      <c r="V7" s="92"/>
-      <c r="W7" s="92"/>
-      <c r="X7" s="92"/>
-      <c r="Y7" s="92"/>
-      <c r="Z7" s="92"/>
-      <c r="AA7" s="92"/>
-      <c r="AB7" s="92"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="81"/>
+      <c r="Q7" s="78"/>
+      <c r="R7" s="79"/>
+      <c r="S7" s="79"/>
+      <c r="T7" s="79"/>
+      <c r="U7" s="79"/>
+      <c r="V7" s="79"/>
+      <c r="W7" s="79"/>
+      <c r="X7" s="79"/>
+      <c r="Y7" s="79"/>
+      <c r="Z7" s="79"/>
+      <c r="AA7" s="79"/>
+      <c r="AB7" s="79"/>
     </row>
     <row r="8" spans="2:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -4015,43 +4015,43 @@
       <c r="D8" s="117"/>
     </row>
     <row r="9" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="96">
+      <c r="C9" s="83">
         <v>0.99</v>
       </c>
-      <c r="D9" s="96">
+      <c r="D9" s="83">
         <v>0.95</v>
       </c>
-      <c r="E9" s="96">
+      <c r="E9" s="83">
         <v>0.9</v>
       </c>
-      <c r="F9" s="96">
+      <c r="F9" s="83">
         <v>0.85</v>
       </c>
-      <c r="G9" s="95" t="s">
+      <c r="G9" s="82" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="97">
+      <c r="B10" s="84">
         <f>104%-0.000000000001</f>
         <v>1.0399999999989999</v>
       </c>
-      <c r="C10" s="96">
+      <c r="C10" s="83">
         <v>1.04</v>
       </c>
-      <c r="D10" s="96">
+      <c r="D10" s="83">
         <v>0.99</v>
       </c>
-      <c r="E10" s="96">
+      <c r="E10" s="83">
         <v>0.95</v>
       </c>
-      <c r="F10" s="96">
+      <c r="F10" s="83">
         <v>0.9</v>
       </c>
-      <c r="G10" s="96">
+      <c r="G10" s="83">
         <v>0.85</v>
       </c>
     </row>
@@ -4063,40 +4063,40 @@
       <c r="D12" s="117"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="95"/>
-      <c r="C13" s="96">
+      <c r="B13" s="82"/>
+      <c r="C13" s="83">
         <v>0.96</v>
       </c>
-      <c r="D13" s="96">
+      <c r="D13" s="83">
         <v>1.01</v>
       </c>
-      <c r="E13" s="96">
+      <c r="E13" s="83">
         <v>1.05</v>
       </c>
-      <c r="F13" s="96">
+      <c r="F13" s="83">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G13" s="95" t="s">
+      <c r="G13" s="82" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="96">
+      <c r="B14" s="83">
         <v>0.96</v>
       </c>
-      <c r="C14" s="96">
+      <c r="C14" s="83">
         <v>1.01</v>
       </c>
-      <c r="D14" s="96">
+      <c r="D14" s="83">
         <v>1.05</v>
       </c>
-      <c r="E14" s="96">
+      <c r="E14" s="83">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F14" s="96">
+      <c r="F14" s="83">
         <v>1.1499999999999999</v>
       </c>
-      <c r="G14" s="96">
+      <c r="G14" s="83">
         <v>1.1499999999999999</v>
       </c>
     </row>

</xml_diff>